<commit_message>
Analysis for Taylor Curtis
of just historical PV installs in the US. created a new module baseline, and a journal file for the analysis.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1F47DE6B-12FD-4BCB-8118-4CA109EB37DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D5E613-FD79-44EF-B957-9198591B2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>“U.S. Solar Market Insight Report: 2012 Year in Review Full Report,” Greentech Media Inc. &amp; SEIA, 2013.</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>Sherwood, 2013</t>
+  </si>
+  <si>
+    <t>c-Si Marketshare</t>
+  </si>
+  <si>
+    <t>All_Marketshare</t>
+  </si>
+  <si>
+    <t>Comm+Utility c-Si PV US Installs</t>
+  </si>
+  <si>
+    <t>PCT of installs</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -239,12 +251,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -268,6 +317,11 @@
     <xf numFmtId="9" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,30 +567,16 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="743194360"/>
-        <c:axId val="743196656"/>
-      </c:scatterChart>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'input-Installs-Subset-CommUtili'!$K$2</c:f>
+              <c:f>'input-Installs-Subset-CommUtili'!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PCT</c:v>
+                  <c:v>Comm+Utility c-Si PV US Installs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -544,7 +584,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -642,87 +682,87 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'input-Installs-Subset-CommUtili'!$K$3:$K$28</c:f>
+              <c:f>'input-Installs-Subset-CommUtili'!$O$3:$O$28</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9.6676666670000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>11.622</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>11.781000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.9449999999999981</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3.4066666666666658</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.52500000000000002</c:v>
+                  <c:v>6.0794999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>11.00166666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.65938864628820959</c:v>
+                  <c:v>28.639666666666653</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57612456747404839</c:v>
+                  <c:v>31.301999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.64885496183206104</c:v>
+                  <c:v>47.821745963399991</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.64011516314779271</c:v>
+                  <c:v>62.388684539559996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.63965087281795519</c:v>
+                  <c:v>95.730302108520007</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.7325060324026198</c:v>
+                  <c:v>197.77909939000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.61379784551913819</c:v>
+                  <c:v>267.47390314270001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.70494853288536619</c:v>
+                  <c:v>507.60275598089197</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.82284129514024529</c:v>
+                  <c:v>1481.2286290301854</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.85089893560969032</c:v>
+                  <c:v>2607.6232262581889</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.83069388701174662</c:v>
+                  <c:v>3353.8843182175783</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.79385719157050227</c:v>
+                  <c:v>2955.3569881658045</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.70895614431880372</c:v>
+                  <c:v>4850.6758664830877</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.82259236143177517</c:v>
+                  <c:v>10615.357717866022</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.78687254978114662</c:v>
+                  <c:v>7777.051848350131</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.77328917803719699</c:v>
+                  <c:v>7243.1254754457032</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.77982783875477768</c:v>
+                  <c:v>8620.7291817664536</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8239738534260812</c:v>
+                  <c:v>13622.949999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,7 +770,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C0E3-4486-81FA-BC2B0BFE102E}"/>
+              <c16:uniqueId val="{00000001-3271-449D-912C-4E5AB9C86484}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -742,8 +782,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="744688992"/>
-        <c:axId val="744690960"/>
+        <c:axId val="743194360"/>
+        <c:axId val="743196656"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="743194360"/>
@@ -913,114 +953,6 @@
         </c:txPr>
         <c:crossAx val="743194360"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="744690960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Percent of Market Commercial &amp; Utility</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="744688992"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="744688992"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="744690960"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1639,16 +1571,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>163513</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>450849</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>30163</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1973,15 +1905,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F9D18A-621B-4AB9-828D-D7D18879DF38}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="O3" sqref="O3:O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="15" max="15" width="8.7265625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2004,8 +1939,14 @@
       <c r="L1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2033,17 +1974,23 @@
       <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1995</v>
       </c>
@@ -2057,18 +2004,25 @@
       <c r="G3" s="5"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3">
+      <c r="J3" s="18">
         <v>12.5</v>
       </c>
       <c r="K3" s="2">
-        <f>E3</f>
+        <f t="shared" ref="K3:K16" si="0">E3</f>
         <v>1</v>
       </c>
       <c r="L3">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <f>J3</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1996</v>
       </c>
@@ -2082,18 +2036,25 @@
       <c r="G4" s="5"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4">
+      <c r="J4" s="18">
         <v>9.6676666670000007</v>
       </c>
       <c r="K4" s="2">
-        <f>E4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L4">
         <v>9.6676666670000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M4">
+        <v>0.99666666666666603</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" ref="O4:O6" si="1">J4</f>
+        <v>9.6676666670000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1997</v>
       </c>
@@ -2107,18 +2068,25 @@
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5">
+      <c r="J5" s="18">
         <v>11.622</v>
       </c>
       <c r="K5" s="2">
-        <f>E5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5">
         <v>11.622</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M5">
+        <v>0.99333333333333296</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="1"/>
+        <v>11.622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1998</v>
       </c>
@@ -2132,18 +2100,25 @@
       <c r="G6" s="5"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6">
+      <c r="J6" s="18">
         <v>11.781000000000001</v>
       </c>
       <c r="K6" s="2">
-        <f>E6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6">
         <v>11.781000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M6">
+        <v>0.99</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="1"/>
+        <v>11.781000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1999</v>
       </c>
@@ -2159,16 +2134,23 @@
       <c r="G7" s="5"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="5">
+      <c r="J7" s="19">
         <f>D7</f>
         <v>3</v>
       </c>
       <c r="K7" s="2">
-        <f>E7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M7">
+        <v>0.98166666666666602</v>
+      </c>
+      <c r="O7" s="3">
+        <f>J7*M7</f>
+        <v>2.9449999999999981</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2000</v>
       </c>
@@ -2188,16 +2170,23 @@
       <c r="G8" s="5"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="5">
-        <f t="shared" ref="J8:J16" si="0">D8</f>
+      <c r="J8" s="19">
+        <f t="shared" ref="J8:J16" si="2">D8</f>
         <v>3.5</v>
       </c>
       <c r="K8" s="2">
-        <f>E8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M8">
+        <v>0.97333333333333305</v>
+      </c>
+      <c r="O8" s="3">
+        <f>J8*M8</f>
+        <v>3.4066666666666658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -2217,16 +2206,23 @@
       <c r="G9" s="5"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="5">
+      <c r="J9" s="19">
+        <f t="shared" si="2"/>
+        <v>6.3</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="0"/>
-        <v>6.3</v>
-      </c>
-      <c r="K9" s="2">
-        <f>E9</f>
         <v>0.52500000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M9">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" ref="O8:O28" si="3">J9*M9</f>
+        <v>6.0794999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -2246,16 +2242,23 @@
       <c r="G10" s="5"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="5">
+      <c r="J10" s="19">
+        <f t="shared" si="2"/>
+        <v>11.5</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="0"/>
-        <v>11.5</v>
-      </c>
-      <c r="K10" s="2">
-        <f>E10</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M10">
+        <v>0.956666666666666</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="3"/>
+        <v>11.00166666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2003</v>
       </c>
@@ -2275,16 +2278,23 @@
       <c r="G11" s="5"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="5">
+      <c r="J11" s="19">
+        <f t="shared" si="2"/>
+        <v>30.199999999999996</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="0"/>
-        <v>30.199999999999996</v>
-      </c>
-      <c r="K11" s="2">
-        <f>E11</f>
         <v>0.65938864628820959</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M11">
+        <v>0.94833333333333303</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="3"/>
+        <v>28.639666666666653</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2004</v>
       </c>
@@ -2304,16 +2314,23 @@
       <c r="G12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="5">
+      <c r="J12" s="19">
+        <f t="shared" si="2"/>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K12" s="2">
         <f t="shared" si="0"/>
-        <v>33.299999999999997</v>
-      </c>
-      <c r="K12" s="2">
-        <f>E12</f>
         <v>0.57612456747404839</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M12">
+        <v>0.94</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="3"/>
+        <v>31.301999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2005</v>
       </c>
@@ -2333,16 +2350,23 @@
       <c r="G13" s="5"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="5">
+      <c r="J13" s="19">
+        <f t="shared" si="2"/>
+        <v>50.999999999999993</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="0"/>
-        <v>50.999999999999993</v>
-      </c>
-      <c r="K13" s="2">
-        <f>E13</f>
         <v>0.64885496183206104</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M13">
+        <v>0.93768129339999995</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="3"/>
+        <v>47.821745963399991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2006</v>
       </c>
@@ -2362,16 +2386,23 @@
       <c r="G14" s="5"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="5">
+      <c r="J14" s="19">
+        <f t="shared" si="2"/>
+        <v>66.7</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="0"/>
-        <v>66.7</v>
-      </c>
-      <c r="K14" s="2">
-        <f>E14</f>
         <v>0.64011516314779271</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M14">
+        <v>0.93536258679999995</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="3"/>
+        <v>62.388684539559996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2007</v>
       </c>
@@ -2391,16 +2422,23 @@
       <c r="G15" s="5"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="5">
+      <c r="J15" s="19">
+        <f t="shared" si="2"/>
+        <v>102.60000000000001</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="0"/>
-        <v>102.60000000000001</v>
-      </c>
-      <c r="K15" s="2">
-        <f>E15</f>
         <v>0.63965087281795519</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M15">
+        <v>0.93304388019999995</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="3"/>
+        <v>95.730302108520007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2008</v>
       </c>
@@ -2420,16 +2458,23 @@
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="5">
+      <c r="J16" s="19">
+        <f t="shared" si="2"/>
+        <v>212.50000000000003</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="0"/>
-        <v>212.50000000000003</v>
-      </c>
-      <c r="K16" s="2">
-        <f>E16</f>
         <v>0.7325060324026198</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M16">
+        <v>0.93072517359999996</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="3"/>
+        <v>197.77909939000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2009</v>
       </c>
@@ -2454,7 +2499,7 @@
         <f>SUM(J3:J17)</f>
         <v>854.270666667</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="19">
         <f>F17</f>
         <v>288.10000000000002</v>
       </c>
@@ -2462,8 +2507,15 @@
         <f>C17</f>
         <v>0.61379784551913819</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M17">
+        <v>0.92840646699999996</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="3"/>
+        <v>267.47390314270001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2010</v>
       </c>
@@ -2487,7 +2539,7 @@
       <c r="I18" s="4">
         <v>0.70494853288536619</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="20">
         <f>H18</f>
         <v>598.38707499999998</v>
       </c>
@@ -2495,8 +2547,15 @@
         <f>I18</f>
         <v>0.70494853288536619</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M18">
+        <v>0.84828495999999998</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" si="3"/>
+        <v>507.60275598089197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -2520,16 +2579,23 @@
       <c r="I19" s="4">
         <v>0.82284129514024529</v>
       </c>
-      <c r="J19" s="4">
-        <f t="shared" ref="J19:J28" si="1">H19</f>
+      <c r="J19" s="20">
+        <f t="shared" ref="J19:J28" si="4">H19</f>
         <v>1596.9187147970001</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" ref="K19:K28" si="2">I19</f>
+        <f t="shared" ref="K19:K28" si="5">I19</f>
         <v>0.82284129514024529</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M19">
+        <v>0.92755418000000001</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" si="3"/>
+        <v>1481.2286290301854</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2012</v>
       </c>
@@ -2553,16 +2619,23 @@
       <c r="I20" s="4">
         <v>0.85089893560969032</v>
       </c>
-      <c r="J20" s="4">
-        <f t="shared" si="1"/>
+      <c r="J20" s="20">
+        <f t="shared" si="4"/>
         <v>2870.8096344149399</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.85089893560969032</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M20">
+        <v>0.90832328100000004</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" si="3"/>
+        <v>2607.6232262581889</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -2580,16 +2653,23 @@
       <c r="I21" s="4">
         <v>0.83069388701174662</v>
       </c>
-      <c r="J21" s="4">
-        <f t="shared" si="1"/>
+      <c r="J21" s="20">
+        <f t="shared" si="4"/>
         <v>3958.9226131057503</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.83069388701174662</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M21">
+        <v>0.84717097200000002</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" si="3"/>
+        <v>3353.8843182175783</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2014</v>
       </c>
@@ -2599,16 +2679,23 @@
       <c r="I22" s="4">
         <v>0.79385719157050227</v>
       </c>
-      <c r="J22" s="4">
-        <f t="shared" si="1"/>
+      <c r="J22" s="20">
+        <f t="shared" si="4"/>
         <v>4957.5187404296503</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79385719157050227</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M22">
+        <v>0.596136322</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" si="3"/>
+        <v>2955.3569881658045</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2015</v>
       </c>
@@ -2618,16 +2705,23 @@
       <c r="I23" s="4">
         <v>0.70895614431880372</v>
       </c>
-      <c r="J23" s="4">
-        <f t="shared" si="1"/>
+      <c r="J23" s="20">
+        <f t="shared" si="4"/>
         <v>5323.5927222003093</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.70895614431880372</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M23">
+        <v>0.91116584599999995</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" si="3"/>
+        <v>4850.6758664830877</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2016</v>
       </c>
@@ -2637,16 +2731,23 @@
       <c r="I24" s="4">
         <v>0.82259236143177517</v>
       </c>
-      <c r="J24" s="4">
-        <f t="shared" si="1"/>
+      <c r="J24" s="20">
+        <f t="shared" si="4"/>
         <v>12424.388969584639</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.82259236143177517</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M24">
+        <v>0.854396763</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="3"/>
+        <v>10615.357717866022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2017</v>
       </c>
@@ -2656,16 +2757,23 @@
       <c r="I25" s="4">
         <v>0.78687254978114662</v>
       </c>
-      <c r="J25" s="4">
-        <f t="shared" si="1"/>
+      <c r="J25" s="20">
+        <f t="shared" si="4"/>
         <v>8718.5985456361705</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.78687254978114662</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M25">
+        <v>0.89200710500000002</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" si="3"/>
+        <v>7777.051848350131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2018</v>
       </c>
@@ -2675,16 +2783,23 @@
       <c r="I26" s="4">
         <v>0.77328917803719699</v>
       </c>
-      <c r="J26" s="4">
-        <f t="shared" si="1"/>
+      <c r="J26" s="20">
+        <f t="shared" si="4"/>
         <v>8317.9550969831307</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.77328917803719699</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M26">
+        <v>0.87078198799999995</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" si="3"/>
+        <v>7243.1254754457032</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -2694,16 +2809,23 @@
       <c r="I27" s="4">
         <v>0.77982783875477768</v>
       </c>
-      <c r="J27" s="4">
-        <f t="shared" si="1"/>
+      <c r="J27" s="20">
+        <f t="shared" si="4"/>
         <v>10538.67695379609</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.77982783875477768</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M27">
+        <v>0.81800867600000005</v>
+      </c>
+      <c r="O27" s="3">
+        <f t="shared" si="3"/>
+        <v>8620.7291817664536</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>2020</v>
       </c>
@@ -2713,18 +2835,26 @@
       <c r="I28" s="4">
         <v>0.8239738534260812</v>
       </c>
-      <c r="J28" s="4">
-        <f t="shared" si="1"/>
+      <c r="J28" s="21">
+        <f t="shared" si="4"/>
         <v>16027</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.8239738534260812</v>
+      </c>
+      <c r="M28">
+        <v>0.85</v>
+      </c>
+      <c r="O28" s="3">
+        <f t="shared" si="3"/>
+        <v>13622.949999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2892,11 +3022,11 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <f>SUM(J8,M8:N8)</f>
+        <f t="shared" ref="O8:O17" si="0">SUM(J8,M8:N8)</f>
         <v>3</v>
       </c>
       <c r="P8" s="12">
-        <f>(M8+N8)/O8</f>
+        <f t="shared" ref="P8:P17" si="1">(M8+N8)/O8</f>
         <v>1</v>
       </c>
     </row>
@@ -2914,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="12">
-        <f>(C9+D9)/SUM(B9:D9)</f>
+        <f t="shared" ref="E9:E21" si="2">(C9+D9)/SUM(B9:D9)</f>
         <v>1</v>
       </c>
       <c r="J9" s="3">
@@ -2933,11 +3063,11 @@
         <v>0.5</v>
       </c>
       <c r="O9">
-        <f>SUM(J9,M9:N9)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="P9" s="12">
-        <f>(M9+N9)/O9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2955,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="12">
-        <f>(C10+D10)/SUM(B10:D10)</f>
+        <f t="shared" si="2"/>
         <v>0.33557046979865773</v>
       </c>
       <c r="J10" s="3">
@@ -2968,19 +3098,19 @@
         <v>12</v>
       </c>
       <c r="M10" s="3">
-        <f>K10-J10</f>
+        <f t="shared" ref="M10:N17" si="3">K10-J10</f>
         <v>2.6000000000000005</v>
       </c>
       <c r="N10" s="3">
-        <f>L10-K10</f>
+        <f t="shared" si="3"/>
         <v>3.6999999999999993</v>
       </c>
       <c r="O10">
-        <f>SUM(J10,M10:N10)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="P10" s="12">
-        <f>(M10+N10)/O10</f>
+        <f t="shared" si="1"/>
         <v>0.52500000000000002</v>
       </c>
     </row>
@@ -2998,7 +3128,7 @@
         <v>9.8999999999999986</v>
       </c>
       <c r="E11" s="12">
-        <f>(C11+D11)/SUM(B11:D11)</f>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J11" s="3">
@@ -3011,19 +3141,19 @@
         <v>23</v>
       </c>
       <c r="M11" s="3">
-        <f>K11-J11</f>
+        <f t="shared" si="3"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="N11" s="3">
-        <f>L11-K11</f>
+        <f t="shared" si="3"/>
         <v>2.6999999999999993</v>
       </c>
       <c r="O11">
-        <f>SUM(J11,M11:N11)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="P11" s="12">
-        <f>(M11+N11)/O11</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3041,7 +3171,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="12">
-        <f>(C12+D12)/SUM(B12:D12)</f>
+        <f t="shared" si="2"/>
         <v>0.60080645161290325</v>
       </c>
       <c r="J12" s="3">
@@ -3054,19 +3184,19 @@
         <v>45.8</v>
       </c>
       <c r="M12" s="3">
-        <f>K12-J12</f>
+        <f t="shared" si="3"/>
         <v>26.6</v>
       </c>
       <c r="N12" s="3">
-        <f>L12-K12</f>
+        <f t="shared" si="3"/>
         <v>3.5999999999999943</v>
       </c>
       <c r="O12">
-        <f>SUM(J12,M12:N12)</f>
+        <f t="shared" si="0"/>
         <v>45.8</v>
       </c>
       <c r="P12" s="12">
-        <f>(M12+N12)/O12</f>
+        <f t="shared" si="1"/>
         <v>0.65938864628820959</v>
       </c>
     </row>
@@ -3084,7 +3214,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="12">
-        <f>(C13+D13)/SUM(B13:D13)</f>
+        <f t="shared" si="2"/>
         <v>0.50084033613445378</v>
       </c>
       <c r="J13" s="3">
@@ -3097,19 +3227,19 @@
         <v>57.8</v>
       </c>
       <c r="M13" s="3">
-        <f>K13-J13</f>
+        <f t="shared" si="3"/>
         <v>31.200000000000003</v>
       </c>
       <c r="N13" s="3">
-        <f>L13-K13</f>
+        <f t="shared" si="3"/>
         <v>2.0999999999999943</v>
       </c>
       <c r="O13">
-        <f>SUM(J13,M13:N13)</f>
+        <f t="shared" si="0"/>
         <v>57.8</v>
       </c>
       <c r="P13" s="12">
-        <f>(M13+N13)/O13</f>
+        <f t="shared" si="1"/>
         <v>0.57612456747404839</v>
       </c>
     </row>
@@ -3127,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="12">
-        <f>(C14+D14)/SUM(B14:D14)</f>
+        <f t="shared" si="2"/>
         <v>0.58837485172004744</v>
       </c>
       <c r="J14" s="3">
@@ -3140,19 +3270,19 @@
         <v>78.599999999999994</v>
       </c>
       <c r="M14" s="3">
-        <f>K14-J14</f>
+        <f t="shared" si="3"/>
         <v>50.999999999999993</v>
       </c>
       <c r="N14" s="3">
-        <f>L14-K14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>SUM(J14,M14:N14)</f>
+        <f t="shared" si="0"/>
         <v>78.599999999999994</v>
       </c>
       <c r="P14" s="12">
-        <f>(M14+N14)/O14</f>
+        <f t="shared" si="1"/>
         <v>0.64885496183206104</v>
       </c>
     </row>
@@ -3170,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="12">
-        <f>(C15+D15)/SUM(B15:D15)</f>
+        <f t="shared" si="2"/>
         <v>0.63577981651376148</v>
       </c>
       <c r="J15" s="3">
@@ -3183,19 +3313,19 @@
         <v>104.2</v>
       </c>
       <c r="M15" s="3">
-        <f>K15-J15</f>
+        <f t="shared" si="3"/>
         <v>66.7</v>
       </c>
       <c r="N15" s="3">
-        <f>L15-K15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f>SUM(J15,M15:N15)</f>
+        <f t="shared" si="0"/>
         <v>104.2</v>
       </c>
       <c r="P15" s="12">
-        <f>(M15+N15)/O15</f>
+        <f t="shared" si="1"/>
         <v>0.64011516314779271</v>
       </c>
     </row>
@@ -3213,7 +3343,7 @@
         <v>14.800000000000011</v>
       </c>
       <c r="E16" s="12">
-        <f>(C16+D16)/SUM(B16:D16)</f>
+        <f t="shared" si="2"/>
         <v>0.64688427299703266</v>
       </c>
       <c r="J16" s="3">
@@ -3226,19 +3356,19 @@
         <v>160.4</v>
       </c>
       <c r="M16" s="3">
-        <f>K16-J16</f>
+        <f t="shared" si="3"/>
         <v>93.2</v>
       </c>
       <c r="N16" s="3">
-        <f>L16-K16</f>
+        <f t="shared" si="3"/>
         <v>9.4000000000000057</v>
       </c>
       <c r="O16">
-        <f>SUM(J16,M16:N16)</f>
+        <f t="shared" si="0"/>
         <v>160.4</v>
       </c>
       <c r="P16" s="12">
-        <f>(M16+N16)/O16</f>
+        <f t="shared" si="1"/>
         <v>0.63965087281795519</v>
       </c>
     </row>
@@ -3256,7 +3386,7 @@
         <v>19.799999999999955</v>
       </c>
       <c r="E17" s="12">
-        <f>(C17+D17)/SUM(B17:D17)</f>
+        <f t="shared" si="2"/>
         <v>0.72123015873015872</v>
       </c>
       <c r="J17" s="3">
@@ -3269,19 +3399,19 @@
         <v>290.10000000000002</v>
       </c>
       <c r="M17" s="3">
-        <f>K17-J17</f>
+        <f t="shared" si="3"/>
         <v>189.6</v>
       </c>
       <c r="N17" s="3">
-        <f>L17-K17</f>
+        <f t="shared" si="3"/>
         <v>22.900000000000034</v>
       </c>
       <c r="O17">
-        <f>SUM(J17,M17:N17)</f>
+        <f t="shared" si="0"/>
         <v>290.10000000000002</v>
       </c>
       <c r="P17" s="12">
-        <f>(M17+N17)/O17</f>
+        <f t="shared" si="1"/>
         <v>0.7325060324026198</v>
       </c>
     </row>
@@ -3299,7 +3429,7 @@
         <v>59.600000000000023</v>
       </c>
       <c r="E18" s="12">
-        <f>(C18+D18)/SUM(B18:D18)</f>
+        <f t="shared" si="2"/>
         <v>0.61379784551913819</v>
       </c>
       <c r="F18" s="16">
@@ -3312,7 +3442,7 @@
         <v>1168.0478000000003</v>
       </c>
       <c r="I18" s="14">
-        <f>(F18+G18)/H18</f>
+        <f t="shared" ref="I18:I29" si="4">(F18+G18)/H18</f>
         <v>0.66880505232748166</v>
       </c>
       <c r="J18" s="3" t="s">
@@ -3370,7 +3500,7 @@
         <v>266</v>
       </c>
       <c r="E19" s="12">
-        <f>(C19+D19)/SUM(B19:D19)</f>
+        <f t="shared" si="2"/>
         <v>0.70990566037735847</v>
       </c>
       <c r="F19">
@@ -3383,7 +3513,7 @@
         <v>848.83796062499994</v>
       </c>
       <c r="I19" s="12">
-        <f>(F19+G19)/H19</f>
+        <f t="shared" si="4"/>
         <v>0.70494853288536619</v>
       </c>
       <c r="Q19">
@@ -3423,7 +3553,7 @@
         <v>760</v>
       </c>
       <c r="E20" s="12">
-        <f>(C20+D20)/SUM(B20:D20)</f>
+        <f t="shared" si="2"/>
         <v>0.83959767072525149</v>
       </c>
       <c r="F20">
@@ -3436,7 +3566,7 @@
         <v>1940.7372044019994</v>
       </c>
       <c r="I20" s="12">
-        <f>(F20+G20)/H20</f>
+        <f t="shared" si="4"/>
         <v>0.82284129514024529</v>
       </c>
       <c r="Q20">
@@ -3476,7 +3606,7 @@
         <v>1782</v>
       </c>
       <c r="E21" s="12">
-        <f>(C21+D21)/SUM(B21:D21)</f>
+        <f t="shared" si="2"/>
         <v>0.85244417622208812</v>
       </c>
       <c r="F21">
@@ -3489,7 +3619,7 @@
         <v>3373.8550070672413</v>
       </c>
       <c r="I21" s="12">
-        <f>(F21+G21)/H21</f>
+        <f t="shared" si="4"/>
         <v>0.85089893560969032</v>
       </c>
       <c r="Q21">
@@ -3532,7 +3662,7 @@
         <v>4765.8020300921853</v>
       </c>
       <c r="I22" s="12">
-        <f>(F22+G22)/H22</f>
+        <f t="shared" si="4"/>
         <v>0.83069388701174662</v>
       </c>
       <c r="Q22">
@@ -3575,7 +3705,7 @@
         <v>6244.8495687519062</v>
       </c>
       <c r="I23" s="12">
-        <f>(F23+G23)/H23</f>
+        <f t="shared" si="4"/>
         <v>0.79385719157050227</v>
       </c>
       <c r="Q23" t="s">
@@ -3602,7 +3732,7 @@
         <v>7509.0578801816455</v>
       </c>
       <c r="I24" s="12">
-        <f>(F24+G24)/H24</f>
+        <f t="shared" si="4"/>
         <v>0.70895614431880372</v>
       </c>
     </row>
@@ -3620,7 +3750,7 @@
         <v>15103.944009350133</v>
       </c>
       <c r="I25" s="12">
-        <f>(F25+G25)/H25</f>
+        <f t="shared" si="4"/>
         <v>0.82259236143177517</v>
       </c>
     </row>
@@ -3638,7 +3768,7 @@
         <v>11080.064424742075</v>
       </c>
       <c r="I26" s="12">
-        <f>(F26+G26)/H26</f>
+        <f t="shared" si="4"/>
         <v>0.78687254978114662</v>
       </c>
     </row>
@@ -3656,7 +3786,7 @@
         <v>10756.590591499287</v>
       </c>
       <c r="I27" s="12">
-        <f>(F27+G27)/H27</f>
+        <f t="shared" si="4"/>
         <v>0.77328917803719699</v>
       </c>
     </row>
@@ -3674,7 +3804,7 @@
         <v>13514.107127316918</v>
       </c>
       <c r="I28" s="12">
-        <f>(F28+G28)/H28</f>
+        <f t="shared" si="4"/>
         <v>0.77982783875477768</v>
       </c>
     </row>
@@ -3692,7 +3822,7 @@
         <v>19450.859919110022</v>
       </c>
       <c r="I29" s="12">
-        <f>(F29+G29)/H29</f>
+        <f t="shared" si="4"/>
         <v>0.8239738534260812</v>
       </c>
     </row>
@@ -3727,11 +3857,11 @@
         <v>9.9</v>
       </c>
       <c r="E38" s="3">
-        <f>C38-B38</f>
+        <f t="shared" ref="E38:E50" si="5">C38-B38</f>
         <v>9.9</v>
       </c>
       <c r="F38" s="3">
-        <f>D38-C38</f>
+        <f t="shared" ref="F38:F50" si="6">D38-C38</f>
         <v>0</v>
       </c>
     </row>
@@ -3749,11 +3879,11 @@
         <v>14.9</v>
       </c>
       <c r="E39" s="3">
-        <f>C39-B39</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="F39" s="3">
-        <f>D39-C39</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3771,11 +3901,11 @@
         <v>29.7</v>
       </c>
       <c r="E40" s="3">
-        <f>C40-B40</f>
+        <f t="shared" si="5"/>
         <v>9.9</v>
       </c>
       <c r="F40" s="3">
-        <f>D40-C40</f>
+        <f t="shared" si="6"/>
         <v>9.8999999999999986</v>
       </c>
     </row>
@@ -3793,11 +3923,11 @@
         <v>49.6</v>
       </c>
       <c r="E41" s="3">
-        <f>C41-B41</f>
+        <f t="shared" si="5"/>
         <v>24.8</v>
       </c>
       <c r="F41" s="3">
-        <f>D41-C41</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -3815,11 +3945,11 @@
         <v>59.5</v>
       </c>
       <c r="E42" s="3">
-        <f>C42-B42</f>
+        <f t="shared" si="5"/>
         <v>29.8</v>
       </c>
       <c r="F42" s="3">
-        <f>D42-C42</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3837,11 +3967,11 @@
         <v>84.3</v>
       </c>
       <c r="E43" s="3">
-        <f>C43-B43</f>
+        <f t="shared" si="5"/>
         <v>49.599999999999994</v>
       </c>
       <c r="F43" s="3">
-        <f>D43-C43</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3859,11 +3989,11 @@
         <v>109</v>
       </c>
       <c r="E44" s="3">
-        <f>C44-B44</f>
+        <f t="shared" si="5"/>
         <v>69.3</v>
       </c>
       <c r="F44" s="3">
-        <f>D44-C44</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3881,11 +4011,11 @@
         <v>168.5</v>
       </c>
       <c r="E45" s="3">
-        <f>C45-B45</f>
+        <f t="shared" si="5"/>
         <v>94.199999999999989</v>
       </c>
       <c r="F45" s="3">
-        <f>D45-C45</f>
+        <f t="shared" si="6"/>
         <v>14.800000000000011</v>
       </c>
     </row>
@@ -3903,11 +4033,11 @@
         <v>302.39999999999998</v>
       </c>
       <c r="E46" s="3">
-        <f>C46-B46</f>
+        <f t="shared" si="5"/>
         <v>198.3</v>
       </c>
       <c r="F46" s="3">
-        <f>D46-C46</f>
+        <f t="shared" si="6"/>
         <v>19.799999999999955</v>
       </c>
     </row>
@@ -3925,11 +4055,11 @@
         <v>436.3</v>
       </c>
       <c r="E47" s="3">
-        <f>C47-B47</f>
+        <f t="shared" si="5"/>
         <v>208.2</v>
       </c>
       <c r="F47" s="3">
-        <f>D47-C47</f>
+        <f t="shared" si="6"/>
         <v>59.600000000000023</v>
       </c>
     </row>
@@ -3947,11 +4077,11 @@
         <v>847.7</v>
       </c>
       <c r="E48" s="11">
-        <f>C48-B48</f>
+        <f t="shared" si="5"/>
         <v>332.1</v>
       </c>
       <c r="F48" s="11">
-        <f>D48-C48</f>
+        <f t="shared" si="6"/>
         <v>267.70000000000005</v>
       </c>
       <c r="G48" s="10">
@@ -3981,11 +4111,11 @@
         <v>1888.8</v>
       </c>
       <c r="E49" s="11">
-        <f>C49-B49</f>
+        <f t="shared" si="5"/>
         <v>823.00000000000011</v>
       </c>
       <c r="F49" s="11">
-        <f>D49-C49</f>
+        <f t="shared" si="6"/>
         <v>763.39999999999986</v>
       </c>
       <c r="G49" s="10">
@@ -4015,11 +4145,11 @@
         <v>3311.6</v>
       </c>
       <c r="E50" s="11">
-        <f>C50-B50</f>
+        <f t="shared" si="5"/>
         <v>1041.1000000000001</v>
       </c>
       <c r="F50" s="11">
-        <f>D50-C50</f>
+        <f t="shared" si="6"/>
         <v>1779.6999999999998</v>
       </c>
       <c r="G50" s="10">

</xml_diff>

<commit_message>
Small Tweaks and tidying
tidying files, small tweaks to journals, will do check of new features on Journal 14 later.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D5E613-FD79-44EF-B957-9198591B2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8231B0-283E-4C28-BDBC-260FA4617975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
+    <workbookView xWindow="32385" yWindow="1005" windowWidth="24615" windowHeight="11910" activeTab="1" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
   </bookViews>
   <sheets>
     <sheet name="input-Installs-Subset-CommUtili" sheetId="1" r:id="rId1"/>
@@ -1907,7 +1907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F9D18A-621B-4AB9-828D-D7D18879DF38}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3:O28"/>
     </sheetView>
   </sheetViews>
@@ -2218,7 +2218,7 @@
         <v>0.96499999999999997</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" ref="O8:O28" si="3">J9*M9</f>
+        <f t="shared" ref="O9:O28" si="3">J9*M9</f>
         <v>6.0794999999999995</v>
       </c>
     </row>
@@ -2862,7 +2862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68613016-2799-46F8-A7F1-1692A33A287D}">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q24" sqref="Q24"/>
     </sheetView>

</xml_diff>

<commit_message>
updates to the historical PV installs calculation
got all scenarios of all pv and just c-Si pv installs working, and simulation runs, playing with graphing and results to come.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94CAA8C-B7F1-4AD2-895F-4128AE695ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339D8A3B-3906-4ADF-A46E-454C782D71FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-8460" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
+    <workbookView xWindow="28680" yWindow="-6405" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
   </bookViews>
   <sheets>
     <sheet name="input-Installs-Subset-CommUtili" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="76">
   <si>
     <t>“U.S. Solar Market Insight Report: 2012 Year in Review Full Report,” Greentech Media Inc. &amp; SEIA, 2013.</t>
   </si>
@@ -227,12 +227,6 @@
     <t>Annual Installs, c-Si [MWdc]</t>
   </si>
   <si>
-    <t>All Sector All Tech Installs [MWdc]</t>
-  </si>
-  <si>
-    <t>All Sector c-Si Installs [MWdc]</t>
-  </si>
-  <si>
     <t>Residential c-Si</t>
   </si>
   <si>
@@ -252,6 +246,24 @@
   </si>
   <si>
     <t>Silicon Marketshare [%]</t>
+  </si>
+  <si>
+    <t>Residential MrktShr</t>
+  </si>
+  <si>
+    <t>Commercial MrktShr</t>
+  </si>
+  <si>
+    <t>Utility MrktShr</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>All Sector All Tech Installs_[MWdc]</t>
+  </si>
+  <si>
+    <t>All Sector c-Si Installs_[MWdc]</t>
   </si>
 </sst>
 </file>
@@ -2814,7 +2826,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>All Sector All Tech Installs [MWdc]</c:v>
+                  <c:v>All Sector All Tech Installs_[MWdc]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3027,7 +3039,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>All Sector c-Si Installs [MWdc]</c:v>
+                  <c:v>All Sector c-Si Installs_[MWdc]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6004,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEC5DA-D656-4E74-BD20-592539DB4636}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6048,7 +6060,7 @@
       <c r="G1" s="27"/>
       <c r="I1"/>
       <c r="J1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K1"/>
       <c r="L1" s="28"/>
@@ -6063,7 +6075,7 @@
       <c r="S1"/>
       <c r="T1"/>
       <c r="U1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="V1"/>
       <c r="W1"/>
@@ -6089,15 +6101,15 @@
         <v>58</v>
       </c>
       <c r="U2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -6109,7 +6121,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>15</v>
@@ -6121,31 +6133,31 @@
         <v>32</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="L3" s="28" t="s">
         <v>32</v>
       </c>
       <c r="M3" s="27" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="N3" t="s">
         <v>32</v>
       </c>
       <c r="P3" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="28" t="s">
-        <v>67</v>
-      </c>
       <c r="S3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="U3" s="28" t="s">
         <v>11</v>
@@ -7699,11 +7711,6 @@
       <c r="S30" s="28">
         <f t="shared" si="5"/>
         <v>18784.548540332304</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="22">
-        <v>2022</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Aluminum Frames Energy Baseline complete
added recycling and remfg energy estimates.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339D8A3B-3906-4ADF-A46E-454C782D71FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6975FCD-8084-4B69-9D0B-DB460879EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-6405" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
   </bookViews>
@@ -3459,6 +3459,1020 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison all Installs,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>c-Si installs, </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SF deployment</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SectorInstalls!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All Sector All Tech Installs_[MWdc]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SectorInstalls!$A$4:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SectorInstalls!$E$4:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>21.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>104.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>290.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>436.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3374</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4766</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6245</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7509</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15104</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11081</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10733</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13511</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19850</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>24095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B99F-42FE-A994-164CB7DD6D2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SectorInstalls!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All Sector c-Si Installs_[MWdc]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SectorInstalls!$A$4:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SectorInstalls!$S$4:$S$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>21.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>78.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>104.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>267.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>406.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1744.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2928.0967741935483</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3706.7922322779177</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3497.9431369436734</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6705.3680714129314</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12597.948399699244</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9620.5165327882023</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9184.9973130760191</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10499.751850031696</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15694.246010785298</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18784.548540332304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B99F-42FE-A994-164CB7DD6D2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>SF deployment curve</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SectorInstalls!$A$33:$A$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SectorInstalls!$B$33:$B$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>1200.6513499999901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2534.3001088299902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2534.3001088299902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5123.0323208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5123.0323208</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9477.5425046750006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9477.5425046750006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9156.77890338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9156.77890338</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16995.842998245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16995.842998245</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4723.5930226999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4723.5930226999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34173.144328415001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34173.144328415001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>73232.04575818</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73232.04575818</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>61963.949007384901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61963.949007384901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>81314.849570865001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>81314.849570865001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>49200.342204749999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>49200.342204749999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>100734.892095405</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>100734.892095405</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>89886.844265459993</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>89886.844265459993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>59996.065785354898</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59996.065785354898</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13613.503684885</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13613.503684885</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36887.263406979997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36887.263406979997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44331.142776660003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44331.142776660003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>71991.796050289995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>71991.796050289995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42648.336863959899</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42648.336863959899</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>69993.457237224997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>69993.457237224997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B99F-42FE-A994-164CB7DD6D2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="959173448"/>
+        <c:axId val="959146224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="959173448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2050"/>
+          <c:min val="1995"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="959146224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="959146224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="959173448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3500,6 +4514,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4571,6 +5625,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4681,6 +6251,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>688067</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>163513</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C38640CC-33AB-40A6-BD51-A564C3908971}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6014,10 +7622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEC5DA-D656-4E74-BD20-592539DB4636}">
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AG73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7716,11 +9324,333 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B32" s="24"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" s="24"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B34" s="24"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="28">
+        <v>2010</v>
+      </c>
+      <c r="B33" s="28">
+        <v>1200.6513499999901</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="28">
+        <v>2011</v>
+      </c>
+      <c r="B34" s="28">
+        <v>2534.3001088299902</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="28">
+        <v>2012</v>
+      </c>
+      <c r="B35" s="28">
+        <v>2534.3001088299902</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="28">
+        <v>2013</v>
+      </c>
+      <c r="B36" s="28">
+        <v>5123.0323208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="28">
+        <v>2014</v>
+      </c>
+      <c r="B37" s="28">
+        <v>5123.0323208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="28">
+        <v>2015</v>
+      </c>
+      <c r="B38" s="28">
+        <v>9477.5425046750006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="28">
+        <v>2016</v>
+      </c>
+      <c r="B39" s="28">
+        <v>9477.5425046750006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="28">
+        <v>2017</v>
+      </c>
+      <c r="B40" s="28">
+        <v>9156.77890338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="28">
+        <v>2018</v>
+      </c>
+      <c r="B41" s="28">
+        <v>9156.77890338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="28">
+        <v>2019</v>
+      </c>
+      <c r="B42" s="28">
+        <v>16995.842998245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="28">
+        <v>2020</v>
+      </c>
+      <c r="B43" s="28">
+        <v>16995.842998245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="28">
+        <v>2021</v>
+      </c>
+      <c r="B44" s="28">
+        <v>4723.5930226999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="28">
+        <v>2022</v>
+      </c>
+      <c r="B45" s="28">
+        <v>4723.5930226999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="28">
+        <v>2023</v>
+      </c>
+      <c r="B46" s="28">
+        <v>34173.144328415001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="28">
+        <v>2024</v>
+      </c>
+      <c r="B47" s="28">
+        <v>34173.144328415001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="28">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="28">
+        <v>73232.04575818</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="28">
+        <v>2026</v>
+      </c>
+      <c r="B49" s="28">
+        <v>73232.04575818</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="28">
+        <v>2027</v>
+      </c>
+      <c r="B50" s="28">
+        <v>61963.949007384901</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="28">
+        <v>2028</v>
+      </c>
+      <c r="B51" s="28">
+        <v>61963.949007384901</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="28">
+        <v>2029</v>
+      </c>
+      <c r="B52" s="28">
+        <v>81314.849570865001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="28">
+        <v>2030</v>
+      </c>
+      <c r="B53" s="28">
+        <v>81314.849570865001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="28">
+        <v>2031</v>
+      </c>
+      <c r="B54" s="28">
+        <v>49200.342204749999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="28">
+        <v>2032</v>
+      </c>
+      <c r="B55" s="28">
+        <v>49200.342204749999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="28">
+        <v>2033</v>
+      </c>
+      <c r="B56" s="28">
+        <v>100734.892095405</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="28">
+        <v>2034</v>
+      </c>
+      <c r="B57" s="28">
+        <v>100734.892095405</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="28">
+        <v>2035</v>
+      </c>
+      <c r="B58" s="28">
+        <v>89886.844265459993</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="28">
+        <v>2036</v>
+      </c>
+      <c r="B59" s="28">
+        <v>89886.844265459993</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="28">
+        <v>2037</v>
+      </c>
+      <c r="B60" s="28">
+        <v>59996.065785354898</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="28">
+        <v>2038</v>
+      </c>
+      <c r="B61" s="28">
+        <v>59996.065785354898</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="28">
+        <v>2039</v>
+      </c>
+      <c r="B62" s="28">
+        <v>13613.503684885</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="28">
+        <v>2040</v>
+      </c>
+      <c r="B63" s="28">
+        <v>13613.503684885</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="28">
+        <v>2041</v>
+      </c>
+      <c r="B64" s="28">
+        <v>36887.263406979997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="28">
+        <v>2042</v>
+      </c>
+      <c r="B65" s="28">
+        <v>36887.263406979997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="28">
+        <v>2043</v>
+      </c>
+      <c r="B66" s="28">
+        <v>44331.142776660003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="28">
+        <v>2044</v>
+      </c>
+      <c r="B67" s="28">
+        <v>44331.142776660003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="28">
+        <v>2045</v>
+      </c>
+      <c r="B68" s="28">
+        <v>71991.796050289995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="28">
+        <v>2046</v>
+      </c>
+      <c r="B69" s="28">
+        <v>71991.796050289995</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="28">
+        <v>2047</v>
+      </c>
+      <c r="B70" s="28">
+        <v>42648.336863959899</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="28">
+        <v>2048</v>
+      </c>
+      <c r="B71" s="28">
+        <v>42648.336863959899</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="28">
+        <v>2049</v>
+      </c>
+      <c r="B72" s="28">
+        <v>69993.457237224997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="28">
+        <v>2050</v>
+      </c>
+      <c r="B73" s="28">
+        <v>69993.457237224997</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Creating Area and Number of modules EQ for Ligia
Added calcs to historical decommissioning journal, and did manipulation of numbers in an excel.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/Calculations-Installs-Subset-CommUtility.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6975FCD-8084-4B69-9D0B-DB460879EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2D113C-91CF-4F36-8B78-24BB738FE0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6405" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{101BAE51-11A4-4817-B77F-32B77C54A859}"/>
   </bookViews>
   <sheets>
     <sheet name="input-Installs-Subset-CommUtili" sheetId="1" r:id="rId1"/>
     <sheet name="SectorInstalls" sheetId="3" r:id="rId2"/>
-    <sheet name="raw and math" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="raw and math" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -497,7 +498,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -524,15 +525,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3752,7 +3750,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B99F-42FE-A994-164CB7DD6D2B}"/>
+              <c16:uniqueId val="{00000000-021A-490C-99C2-97C8313D0967}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3965,7 +3963,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B99F-42FE-A994-164CB7DD6D2B}"/>
+              <c16:uniqueId val="{00000001-021A-490C-99C2-97C8313D0967}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3989,7 +3987,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SectorInstalls!$A$33:$A$73</c:f>
+              <c:f>Sheet1!$A$1:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -4121,7 +4119,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SectorInstalls!$B$33:$B$73</c:f>
+              <c:f>Sheet1!$B$1:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -4254,7 +4252,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B99F-42FE-A994-164CB7DD6D2B}"/>
+              <c16:uniqueId val="{00000002-021A-490C-99C2-97C8313D0967}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6187,15 +6185,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>177799</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>377825</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6256,25 +6254,30 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>688067</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>163513</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>535667</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C38640CC-33AB-40A6-BD51-A564C3908971}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C318EED9-651C-4AC0-BC17-5307B9325B8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6288,7 +6291,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6602,7 +6605,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.7265625" style="22"/>
     <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7265625" style="2"/>
@@ -6814,7 +6816,7 @@
       <c r="A7">
         <v>1999</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7">
         <v>17.200000000000003</v>
       </c>
       <c r="C7" s="6"/>
@@ -6849,7 +6851,7 @@
       <c r="A8">
         <v>2000</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8">
         <v>21.5</v>
       </c>
       <c r="C8" s="6">
@@ -6888,7 +6890,7 @@
       <c r="A9">
         <v>2001</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9">
         <v>29</v>
       </c>
       <c r="C9" s="6">
@@ -6927,7 +6929,7 @@
       <c r="A10">
         <v>2002</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10">
         <v>44.4</v>
       </c>
       <c r="C10" s="6">
@@ -6966,7 +6968,7 @@
       <c r="A11">
         <v>2003</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11">
         <v>63</v>
       </c>
       <c r="C11" s="6">
@@ -7005,7 +7007,7 @@
       <c r="A12">
         <v>2004</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12">
         <v>100.8</v>
       </c>
       <c r="C12" s="6">
@@ -7044,7 +7046,7 @@
       <c r="A13">
         <v>2005</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13">
         <v>103</v>
       </c>
       <c r="C13" s="6">
@@ -7083,7 +7085,7 @@
       <c r="A14">
         <v>2006</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14">
         <v>144</v>
       </c>
       <c r="C14" s="6">
@@ -7122,7 +7124,7 @@
       <c r="A15">
         <v>2007</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15">
         <v>207.5</v>
       </c>
       <c r="C15" s="6">
@@ -7161,7 +7163,7 @@
       <c r="A16">
         <v>2008</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16">
         <v>338</v>
       </c>
       <c r="C16" s="6">
@@ -7200,7 +7202,7 @@
       <c r="A17">
         <v>2009</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17">
         <v>790.09999999999991</v>
       </c>
       <c r="C17" s="6">
@@ -7244,7 +7246,7 @@
       <c r="A18">
         <v>2010</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18">
         <v>960.40000000000009</v>
       </c>
       <c r="C18" s="6">
@@ -7580,7 +7582,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="22">
+      <c r="A29">
         <v>2021</v>
       </c>
       <c r="I29" s="3">
@@ -7599,17 +7601,17 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="22">
+      <c r="A30">
         <v>2022</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="22">
+      <c r="A31">
         <v>2023</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="22">
+      <c r="A32">
         <v>2024</v>
       </c>
     </row>
@@ -7622,26 +7624,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEC5DA-D656-4E74-BD20-592539DB4636}">
-  <dimension ref="A1:AG73"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.7265625" style="27" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.90625" customWidth="1"/>
     <col min="9" max="9" width="12.08984375" customWidth="1"/>
     <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="28" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.453125" customWidth="1"/>
     <col min="15" max="15" width="2" customWidth="1"/>
@@ -7659,46 +7661,21 @@
     <col min="27" max="27" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="I1"/>
       <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="K1"/>
-      <c r="L1" s="28"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
       <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
       <c r="U1" t="s">
         <v>66</v>
       </c>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-      <c r="AB1"/>
-      <c r="AC1"/>
-      <c r="AD1"/>
-      <c r="AE1"/>
-      <c r="AF1"/>
-      <c r="AG1"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>61</v>
       </c>
@@ -7715,8 +7692,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>73</v>
       </c>
       <c r="B3" t="s">
@@ -7728,10 +7705,10 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
@@ -7740,79 +7717,79 @@
       <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" t="s">
         <v>71</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" t="s">
         <v>72</v>
       </c>
       <c r="N3" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" t="s">
         <v>63</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="R3" t="s">
         <v>65</v>
       </c>
       <c r="S3" t="s">
         <v>75</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="U3" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="28" t="s">
+      <c r="V3" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="28" t="s">
+      <c r="W3" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="28" t="s">
+      <c r="X3" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="28" t="s">
+      <c r="Y3" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="28" t="s">
+      <c r="Z3" t="s">
         <v>9</v>
       </c>
       <c r="AA3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A4" s="22">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>1995</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="27">
+      <c r="C4" s="27"/>
+      <c r="D4">
         <v>12</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4">
         <f>SUM(B4:D4)</f>
         <v>21.7</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4">
         <f t="shared" ref="G4:G18" si="0">SUM(C4:D4)</f>
         <v>12</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4">
         <f t="shared" ref="H4:H18" si="1">SUM(B4:D4)</f>
         <v>21.7</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" t="s">
         <v>44</v>
       </c>
       <c r="J4">
@@ -7827,12 +7804,12 @@
       <c r="N4" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="30">
+      <c r="P4" s="27">
         <f>B4*J4</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="28">
+      <c r="Q4" s="27"/>
+      <c r="R4">
         <f t="shared" ref="R4:R8" si="2">D4*M4</f>
         <v>12</v>
       </c>
@@ -7841,155 +7818,155 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A5" s="22">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>1996</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="27">
         <v>1.3000000000000007</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="27">
+      <c r="C5" s="27"/>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5">
         <f t="shared" ref="E5:E29" si="3">SUM(B5:D5)</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>1.3000000000000007</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="27">
         <f t="shared" ref="P5:P7" si="4">B5*J5</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="28">
+      <c r="Q5" s="27"/>
+      <c r="R5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S5" s="28">
+      <c r="S5">
         <f t="shared" ref="S5:S30" si="5">SUM(P5:R5)</f>
         <v>1.3000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A6" s="22">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>1997</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="27">
         <v>2.6999999999999993</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="27">
+      <c r="C6" s="27"/>
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6">
         <f t="shared" si="3"/>
         <v>2.6999999999999993</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>2.6999999999999993</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="27">
         <f t="shared" si="4"/>
         <v>2.6999999999999993</v>
       </c>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="28">
+      <c r="Q6" s="27"/>
+      <c r="R6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S6" s="28">
+      <c r="S6">
         <f t="shared" si="5"/>
         <v>2.6999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A7" s="22">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>1998</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="27">
         <v>2.2000000000000011</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="27">
+      <c r="C7" s="27"/>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7">
         <f t="shared" si="3"/>
         <v>2.2000000000000011</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>2.2000000000000011</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7">
         <v>1</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="P7" s="30">
+      <c r="P7" s="27">
         <f t="shared" si="4"/>
         <v>2.2000000000000011</v>
       </c>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28">
+      <c r="Q7" s="27"/>
+      <c r="R7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7">
         <f t="shared" si="5"/>
         <v>2.2000000000000011</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A8" s="22">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>1999</v>
       </c>
       <c r="B8">
@@ -8001,49 +7978,49 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8">
         <v>1</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8">
         <v>1</v>
       </c>
       <c r="P8">
         <f>B8*J8</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="28">
+      <c r="Q8">
         <f>C8*K8</f>
         <v>3</v>
       </c>
-      <c r="R8" s="28">
+      <c r="R8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S8" s="28">
+      <c r="S8">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A9" s="22">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>2000</v>
       </c>
       <c r="B9">
@@ -8055,49 +8032,49 @@
       <c r="D9">
         <v>0.6</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9">
         <f t="shared" si="3"/>
         <v>3.6</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9">
         <f>SUM(C9:D9)</f>
         <v>3.6</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>3.6</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9">
         <v>1</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="P9" s="28">
+      <c r="P9">
         <f t="shared" ref="P9:P30" si="6">B9*J9</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="28">
+      <c r="Q9">
         <f t="shared" ref="Q9:Q30" si="7">C9*K9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="28">
+      <c r="R9">
         <f t="shared" ref="R9:R30" si="8">D9*M9</f>
         <v>0.6</v>
       </c>
-      <c r="S9" s="28">
+      <c r="S9">
         <f t="shared" si="5"/>
         <v>3.6</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A10" s="22">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>2001</v>
       </c>
       <c r="B10">
@@ -8109,49 +8086,49 @@
       <c r="D10">
         <v>3.6999999999999993</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10">
         <v>1</v>
       </c>
-      <c r="M10" s="28">
+      <c r="M10">
         <v>1</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10">
         <f t="shared" si="6"/>
         <v>5.7</v>
       </c>
-      <c r="Q10" s="28">
+      <c r="Q10">
         <f t="shared" si="7"/>
         <v>2.6000000000000005</v>
       </c>
-      <c r="R10" s="28">
+      <c r="R10">
         <f t="shared" si="8"/>
         <v>3.6999999999999993</v>
       </c>
-      <c r="S10" s="28">
+      <c r="S10">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A11" s="22">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>2002</v>
       </c>
       <c r="B11">
@@ -8163,49 +8140,49 @@
       <c r="D11">
         <v>2.6999999999999993</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11">
         <f>SUM(B11:D11)</f>
         <v>23</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M11">
         <v>1</v>
       </c>
-      <c r="P11" s="28">
+      <c r="P11">
         <f t="shared" si="6"/>
         <v>11.5</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="Q11">
         <f t="shared" si="7"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="R11" s="28">
+      <c r="R11">
         <f t="shared" si="8"/>
         <v>2.6999999999999993</v>
       </c>
-      <c r="S11" s="28">
+      <c r="S11">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A12" s="22">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>2003</v>
       </c>
       <c r="B12">
@@ -8217,49 +8194,49 @@
       <c r="D12">
         <v>3.5999999999999943</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12">
         <f t="shared" si="3"/>
         <v>45.8</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>30.199999999999996</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12">
         <f t="shared" si="1"/>
         <v>45.8</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12">
         <v>1</v>
       </c>
-      <c r="M12" s="28">
+      <c r="M12">
         <v>1</v>
       </c>
-      <c r="P12" s="28">
+      <c r="P12">
         <f t="shared" si="6"/>
         <v>15.6</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="Q12">
         <f t="shared" si="7"/>
         <v>26.6</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12">
         <f t="shared" si="8"/>
         <v>3.5999999999999943</v>
       </c>
-      <c r="S12" s="28">
+      <c r="S12">
         <f t="shared" si="5"/>
         <v>45.8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A13" s="22">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>2004</v>
       </c>
       <c r="B13">
@@ -8271,49 +8248,49 @@
       <c r="D13">
         <v>2.0999999999999943</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13">
         <f t="shared" si="3"/>
         <v>57.8</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>33.299999999999997</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13">
         <f t="shared" si="1"/>
         <v>57.8</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13">
         <v>1</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13">
         <f t="shared" si="6"/>
         <v>24.5</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="Q13">
         <f t="shared" si="7"/>
         <v>31.200000000000003</v>
       </c>
-      <c r="R13" s="28">
+      <c r="R13">
         <f t="shared" si="8"/>
         <v>2.0999999999999943</v>
       </c>
-      <c r="S13" s="28">
+      <c r="S13">
         <f t="shared" si="5"/>
         <v>57.8</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A14" s="22">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>2005</v>
       </c>
       <c r="B14">
@@ -8325,49 +8302,49 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14">
         <f t="shared" si="3"/>
         <v>78.599999999999994</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14">
         <f t="shared" si="0"/>
         <v>50.999999999999993</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>78.599999999999994</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14">
         <v>1</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14">
         <v>1</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14">
         <v>1</v>
       </c>
-      <c r="P14" s="28">
+      <c r="P14">
         <f t="shared" si="6"/>
         <v>27.6</v>
       </c>
-      <c r="Q14" s="28">
+      <c r="Q14">
         <f t="shared" si="7"/>
         <v>50.999999999999993</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S14" s="28">
+      <c r="S14">
         <f t="shared" si="5"/>
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A15" s="22">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>2006</v>
       </c>
       <c r="B15">
@@ -8379,49 +8356,49 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15">
         <f t="shared" si="3"/>
         <v>104.2</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15">
         <f t="shared" si="0"/>
         <v>66.7</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>104.2</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" t="s">
         <v>1</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15">
         <v>1</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15">
         <v>1</v>
       </c>
-      <c r="M15" s="28">
+      <c r="M15">
         <v>1</v>
       </c>
-      <c r="P15" s="28">
+      <c r="P15">
         <f t="shared" si="6"/>
         <v>37.5</v>
       </c>
-      <c r="Q15" s="28">
+      <c r="Q15">
         <f t="shared" si="7"/>
         <v>66.7</v>
       </c>
-      <c r="R15" s="28">
+      <c r="R15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S15" s="28">
+      <c r="S15">
         <f t="shared" si="5"/>
         <v>104.2</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A16" s="22">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>2007</v>
       </c>
       <c r="B16">
@@ -8433,52 +8410,52 @@
       <c r="D16">
         <v>9.4000000000000057</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16">
         <f t="shared" si="3"/>
         <v>160.4</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16">
         <f t="shared" si="0"/>
         <v>102.60000000000001</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>160.4</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16">
         <v>1</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
-      <c r="N16" s="28" t="s">
+      <c r="N16" t="s">
         <v>49</v>
       </c>
-      <c r="P16" s="28">
+      <c r="P16">
         <f t="shared" si="6"/>
         <v>57.8</v>
       </c>
-      <c r="Q16" s="28">
+      <c r="Q16">
         <f t="shared" si="7"/>
         <v>93.2</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16">
         <f t="shared" si="8"/>
         <v>9.4000000000000057</v>
       </c>
-      <c r="S16" s="28">
+      <c r="S16">
         <f t="shared" si="5"/>
         <v>160.4</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="22">
+      <c r="A17">
         <v>2008</v>
       </c>
       <c r="B17">
@@ -8490,52 +8467,52 @@
       <c r="D17">
         <v>22.900000000000034</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17">
         <f t="shared" si="3"/>
         <v>290.10000000000002</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17">
         <f>SUM(C17:D17)</f>
         <v>212.50000000000003</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>290.10000000000002</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" t="s">
         <v>1</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17">
         <v>1</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17" s="28" t="s">
+      <c r="N17" t="s">
         <v>49</v>
       </c>
-      <c r="P17" s="28">
+      <c r="P17">
         <f t="shared" si="6"/>
         <v>77.599999999999994</v>
       </c>
-      <c r="Q17" s="28">
+      <c r="Q17">
         <f t="shared" si="7"/>
         <v>189.6</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S17" s="28">
+      <c r="S17">
         <f t="shared" si="5"/>
         <v>267.2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="22">
+      <c r="A18">
         <v>2009</v>
       </c>
       <c r="B18" s="12">
@@ -8547,68 +8524,68 @@
       <c r="D18" s="12">
         <v>59.600000000000023</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18">
         <f t="shared" si="3"/>
         <v>436.3</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18">
         <f t="shared" si="0"/>
         <v>267.8</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>436.3</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="I18" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J18">
         <v>1</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18">
         <v>1</v>
       </c>
       <c r="M18">
         <v>0.5</v>
       </c>
-      <c r="N18" s="28" t="s">
+      <c r="N18" t="s">
         <v>49</v>
       </c>
-      <c r="P18" s="28">
+      <c r="P18">
         <f t="shared" si="6"/>
         <v>168.5</v>
       </c>
-      <c r="Q18" s="28">
+      <c r="Q18">
         <f t="shared" si="7"/>
         <v>208.2</v>
       </c>
-      <c r="R18" s="28">
+      <c r="R18">
         <f t="shared" si="8"/>
         <v>29.800000000000011</v>
       </c>
-      <c r="S18" s="28">
+      <c r="S18">
         <f t="shared" si="5"/>
         <v>406.5</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="22">
+      <c r="A19">
         <v>2010</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19">
         <v>246</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19">
         <v>337</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19">
         <v>267</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19">
         <f t="shared" si="3"/>
         <v>850</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19">
         <f>SUM(C19:D19)</f>
         <v>604</v>
       </c>
@@ -8622,174 +8599,174 @@
       <c r="J19">
         <v>1</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K19">
         <v>1</v>
       </c>
       <c r="M19">
         <v>0.33333333333333331</v>
       </c>
-      <c r="N19" s="28" t="s">
+      <c r="N19" t="s">
         <v>49</v>
       </c>
-      <c r="P19" s="28">
+      <c r="P19">
         <f t="shared" si="6"/>
         <v>246</v>
       </c>
-      <c r="Q19" s="28">
+      <c r="Q19">
         <f t="shared" si="7"/>
         <v>337</v>
       </c>
-      <c r="R19" s="28">
+      <c r="R19">
         <f t="shared" si="8"/>
         <v>89</v>
       </c>
-      <c r="S19" s="28">
+      <c r="S19">
         <f t="shared" si="5"/>
         <v>672</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="22">
+      <c r="A20">
         <v>2011</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20">
         <v>305</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20">
         <v>850</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20">
         <v>786</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20">
         <f t="shared" si="3"/>
         <v>1941</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20">
         <f t="shared" ref="G20:G30" si="9">SUM(C20:D20)</f>
         <v>1636</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20">
         <f t="shared" ref="H20:H30" si="10">SUM(B20:D20)</f>
         <v>1941</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" t="s">
         <v>33</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20">
         <v>1</v>
       </c>
       <c r="M20">
         <v>0.75</v>
       </c>
-      <c r="N20" s="28" t="s">
+      <c r="N20" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="28">
+      <c r="P20">
         <f t="shared" si="6"/>
         <v>305</v>
       </c>
-      <c r="Q20" s="28">
+      <c r="Q20">
         <f t="shared" si="7"/>
         <v>850</v>
       </c>
-      <c r="R20" s="28">
+      <c r="R20">
         <f t="shared" si="8"/>
         <v>589.5</v>
       </c>
-      <c r="S20" s="28">
+      <c r="S20">
         <f t="shared" si="5"/>
         <v>1744.5</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="22">
+      <c r="A21">
         <v>2012</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21">
         <v>496</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="23">
         <v>1075</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="23">
         <v>1803</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21">
         <f t="shared" si="3"/>
         <v>3374</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="27">
+      <c r="F21" s="23"/>
+      <c r="G21">
         <f t="shared" si="9"/>
         <v>2878</v>
       </c>
-      <c r="H21" s="27">
+      <c r="H21">
         <f t="shared" si="10"/>
         <v>3374</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" t="s">
         <v>33</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21">
         <v>1</v>
       </c>
       <c r="M21">
         <v>0.75268817204301086</v>
       </c>
-      <c r="N21" s="28" t="s">
+      <c r="N21" t="s">
         <v>49</v>
       </c>
-      <c r="P21" s="28">
+      <c r="P21">
         <f t="shared" si="6"/>
         <v>496</v>
       </c>
-      <c r="Q21" s="28">
+      <c r="Q21">
         <f t="shared" si="7"/>
         <v>1075</v>
       </c>
-      <c r="R21" s="28">
+      <c r="R21">
         <f t="shared" si="8"/>
         <v>1357.0967741935485</v>
       </c>
-      <c r="S21" s="28">
+      <c r="S21">
         <f t="shared" si="5"/>
         <v>2928.0967741935483</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="22">
+      <c r="A22">
         <v>2013</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22">
         <v>799</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="23">
         <v>1109</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>2858</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22">
         <f t="shared" si="3"/>
         <v>4766</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="27">
+      <c r="F22" s="23"/>
+      <c r="G22">
         <f t="shared" si="9"/>
         <v>3967</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22">
         <f t="shared" si="10"/>
         <v>4766</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" t="s">
         <v>33</v>
       </c>
       <c r="J22">
@@ -8805,53 +8782,53 @@
       <c r="M22">
         <v>0.62962962962962965</v>
       </c>
-      <c r="N22" s="28" t="s">
+      <c r="N22" t="s">
         <v>49</v>
       </c>
-      <c r="P22" s="28">
+      <c r="P22">
         <f t="shared" si="6"/>
         <v>799</v>
       </c>
-      <c r="Q22" s="28">
+      <c r="Q22">
         <f t="shared" si="7"/>
         <v>1108.310750796436</v>
       </c>
-      <c r="R22" s="28">
+      <c r="R22">
         <f t="shared" si="8"/>
         <v>1799.4814814814815</v>
       </c>
-      <c r="S22" s="28">
+      <c r="S22">
         <f t="shared" si="5"/>
         <v>3706.7922322779177</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="22">
+      <c r="A23">
         <v>2014</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="23">
         <v>1268</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="23">
         <v>1055</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="23">
         <v>3922</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23">
         <f t="shared" si="3"/>
         <v>6245</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="27">
+      <c r="F23" s="23"/>
+      <c r="G23">
         <f t="shared" si="9"/>
         <v>4977</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23">
         <f t="shared" si="10"/>
         <v>6245</v>
       </c>
-      <c r="I23" s="27" t="s">
+      <c r="I23" t="s">
         <v>33</v>
       </c>
       <c r="J23">
@@ -8861,59 +8838,59 @@
         <f>1-0.000397762162618945</f>
         <v>0.999602237837381</v>
       </c>
-      <c r="L23" s="28" t="s">
+      <c r="L23" t="s">
         <v>47</v>
       </c>
       <c r="M23">
         <v>0.29968454258675081</v>
       </c>
-      <c r="N23" s="28" t="s">
+      <c r="N23" t="s">
         <v>49</v>
       </c>
-      <c r="P23" s="28">
+      <c r="P23">
         <f t="shared" si="6"/>
         <v>1268</v>
       </c>
-      <c r="Q23" s="28">
+      <c r="Q23">
         <f t="shared" si="7"/>
         <v>1054.580360918437</v>
       </c>
-      <c r="R23" s="28">
+      <c r="R23">
         <f t="shared" si="8"/>
         <v>1175.3627760252366</v>
       </c>
-      <c r="S23" s="28">
+      <c r="S23">
         <f t="shared" si="5"/>
         <v>3497.9431369436734</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="22">
+      <c r="A24">
         <v>2015</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="23">
         <v>2171</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="23">
         <v>1070</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <v>4268</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24">
         <f t="shared" si="3"/>
         <v>7509</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="27">
+      <c r="F24" s="23"/>
+      <c r="G24">
         <f t="shared" si="9"/>
         <v>5338</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24">
         <f t="shared" si="10"/>
         <v>7509</v>
       </c>
-      <c r="I24" s="27" t="s">
+      <c r="I24" t="s">
         <v>33</v>
       </c>
       <c r="J24">
@@ -8923,59 +8900,59 @@
         <f>1-0.000554767346668965</f>
         <v>0.99944523265333107</v>
       </c>
-      <c r="L24" s="28" t="s">
+      <c r="L24" t="s">
         <v>47</v>
       </c>
       <c r="M24">
         <v>0.81184668989547037</v>
       </c>
-      <c r="N24" s="28" t="s">
+      <c r="N24" t="s">
         <v>49</v>
       </c>
-      <c r="P24" s="28">
+      <c r="P24">
         <f t="shared" si="6"/>
         <v>2171</v>
       </c>
-      <c r="Q24" s="28">
+      <c r="Q24">
         <f t="shared" si="7"/>
         <v>1069.4063989390643</v>
       </c>
-      <c r="R24" s="28">
+      <c r="R24">
         <f t="shared" si="8"/>
         <v>3464.9616724738676</v>
       </c>
-      <c r="S24" s="28">
+      <c r="S24">
         <f t="shared" si="5"/>
         <v>6705.3680714129314</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="22">
+      <c r="A25">
         <v>2016</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="23">
         <v>2638</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="23">
         <v>1715</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <v>10751</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25">
         <f t="shared" si="3"/>
         <v>15104</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="27">
+      <c r="F25" s="23"/>
+      <c r="G25">
         <f t="shared" si="9"/>
         <v>12466</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25">
         <f t="shared" si="10"/>
         <v>15104</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" t="s">
         <v>33</v>
       </c>
       <c r="J25">
@@ -8985,59 +8962,59 @@
         <f>1-0.00358897663231095</f>
         <v>0.99641102336768905</v>
       </c>
-      <c r="L25" s="28" t="s">
+      <c r="L25" t="s">
         <v>47</v>
       </c>
       <c r="M25">
         <v>0.76747311827956999</v>
       </c>
-      <c r="N25" s="28" t="s">
+      <c r="N25" t="s">
         <v>49</v>
       </c>
-      <c r="P25" s="28">
+      <c r="P25">
         <f t="shared" si="6"/>
         <v>2638</v>
       </c>
-      <c r="Q25" s="28">
+      <c r="Q25">
         <f t="shared" si="7"/>
         <v>1708.8449050755867</v>
       </c>
-      <c r="R25" s="28">
+      <c r="R25">
         <f t="shared" si="8"/>
         <v>8251.1034946236578</v>
       </c>
-      <c r="S25" s="28">
+      <c r="S25">
         <f t="shared" si="5"/>
         <v>12597.948399699244</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="22">
+      <c r="A26">
         <v>2017</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="23">
         <v>2239</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="23">
         <v>2366</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="23">
         <v>6476</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26">
         <f t="shared" si="3"/>
         <v>11081</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="27">
+      <c r="F26" s="23"/>
+      <c r="G26">
         <f t="shared" si="9"/>
         <v>8842</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26">
         <f t="shared" si="10"/>
         <v>11081</v>
       </c>
-      <c r="I26" s="27" t="s">
+      <c r="I26" t="s">
         <v>33</v>
       </c>
       <c r="J26">
@@ -9047,59 +9024,59 @@
         <f>1-0.00679691734044147</f>
         <v>0.99320308265955848</v>
       </c>
-      <c r="L26" s="28" t="s">
+      <c r="L26" t="s">
         <v>47</v>
       </c>
       <c r="M26">
         <v>0.77696078431372551</v>
       </c>
-      <c r="N26" s="28" t="s">
+      <c r="N26" t="s">
         <v>49</v>
       </c>
-      <c r="P26" s="28">
+      <c r="P26">
         <f t="shared" si="6"/>
         <v>2239</v>
       </c>
-      <c r="Q26" s="28">
+      <c r="Q26">
         <f t="shared" si="7"/>
         <v>2349.9184935725152</v>
       </c>
-      <c r="R26" s="28">
+      <c r="R26">
         <f t="shared" si="8"/>
         <v>5031.5980392156862</v>
       </c>
-      <c r="S26" s="28">
+      <c r="S26">
         <f t="shared" si="5"/>
         <v>9620.5165327882023</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="22">
+      <c r="A27">
         <v>2018</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="23">
         <v>2418</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="23">
         <v>2196</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <v>6119</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27">
         <f t="shared" si="3"/>
         <v>10733</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="27">
+      <c r="F27" s="23"/>
+      <c r="G27">
         <f t="shared" si="9"/>
         <v>8315</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27">
         <f t="shared" si="10"/>
         <v>10733</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" t="s">
         <v>33</v>
       </c>
       <c r="J27">
@@ -9109,59 +9086,59 @@
         <f>1-0.0100664669777662</f>
         <v>0.98993353302223375</v>
       </c>
-      <c r="L27" s="28" t="s">
+      <c r="L27" t="s">
         <v>47</v>
       </c>
       <c r="M27">
         <v>0.75062972292191443</v>
       </c>
-      <c r="N27" s="28" t="s">
+      <c r="N27" t="s">
         <v>49</v>
       </c>
-      <c r="P27" s="28">
+      <c r="P27">
         <f t="shared" si="6"/>
         <v>2418</v>
       </c>
-      <c r="Q27" s="28">
+      <c r="Q27">
         <f t="shared" si="7"/>
         <v>2173.8940385168253</v>
       </c>
-      <c r="R27" s="28">
+      <c r="R27">
         <f t="shared" si="8"/>
         <v>4593.1032745591947</v>
       </c>
-      <c r="S27" s="28">
+      <c r="S27">
         <f t="shared" si="5"/>
         <v>9184.9973130760191</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="22">
+      <c r="A28">
         <v>2019</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="23">
         <v>2865</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="23">
         <v>2184</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <v>8462</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28">
         <f t="shared" si="3"/>
         <v>13511</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="27">
+      <c r="F28" s="23"/>
+      <c r="G28">
         <f t="shared" si="9"/>
         <v>10646</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28">
         <f t="shared" si="10"/>
         <v>13511</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I28" t="s">
         <v>33</v>
       </c>
       <c r="J28">
@@ -9171,59 +9148,59 @@
         <f>1-0.000414568122519654</f>
         <v>0.99958543187748039</v>
       </c>
-      <c r="L28" s="28" t="s">
+      <c r="L28" t="s">
         <v>47</v>
       </c>
       <c r="M28">
         <v>0.64425162689804771</v>
       </c>
-      <c r="N28" s="28" t="s">
+      <c r="N28" t="s">
         <v>49</v>
       </c>
-      <c r="P28" s="28">
+      <c r="P28">
         <f>B28*J28</f>
         <v>2865</v>
       </c>
-      <c r="Q28" s="28">
+      <c r="Q28">
         <f t="shared" si="7"/>
         <v>2183.094583220417</v>
       </c>
-      <c r="R28" s="28">
+      <c r="R28">
         <f t="shared" si="8"/>
         <v>5451.6572668112794</v>
       </c>
-      <c r="S28" s="28">
+      <c r="S28">
         <f t="shared" si="5"/>
         <v>10499.751850031696</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="22">
+      <c r="A29">
         <v>2020</v>
       </c>
-      <c r="B29" s="24">
+      <c r="B29" s="23">
         <v>3242</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="23">
         <v>2347</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <v>14261</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29">
         <f t="shared" si="3"/>
         <v>19850</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="27">
+      <c r="F29" s="23"/>
+      <c r="G29">
         <f t="shared" si="9"/>
         <v>16608</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29">
         <f t="shared" si="10"/>
         <v>19850</v>
       </c>
-      <c r="I29" s="27" t="s">
+      <c r="I29" t="s">
         <v>33</v>
       </c>
       <c r="J29">
@@ -9233,59 +9210,59 @@
         <f>1-0.00210616889812066</f>
         <v>0.99789383110187935</v>
       </c>
-      <c r="L29" s="28" t="s">
+      <c r="L29" t="s">
         <v>47</v>
       </c>
       <c r="M29">
         <v>0.70893970893970881</v>
       </c>
-      <c r="N29" s="28" t="s">
+      <c r="N29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="28">
+      <c r="P29">
         <f t="shared" si="6"/>
         <v>3242</v>
       </c>
-      <c r="Q29" s="28">
+      <c r="Q29">
         <f t="shared" si="7"/>
         <v>2342.0568215961107</v>
       </c>
-      <c r="R29" s="28">
+      <c r="R29">
         <f t="shared" si="8"/>
         <v>10110.189189189188</v>
       </c>
-      <c r="S29" s="28">
+      <c r="S29">
         <f t="shared" si="5"/>
         <v>15694.246010785298</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="22">
+      <c r="A30">
         <v>2021</v>
       </c>
-      <c r="B30" s="24">
+      <c r="B30" s="23">
         <v>4252</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>2679</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>17164</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="23">
         <f>SUM(B30:D30)</f>
         <v>24095</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="27">
+      <c r="F30" s="23"/>
+      <c r="G30">
         <f t="shared" si="9"/>
         <v>19843</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30">
         <f t="shared" si="10"/>
         <v>24095</v>
       </c>
-      <c r="I30" s="27" t="s">
+      <c r="I30" t="s">
         <v>48</v>
       </c>
       <c r="J30">
@@ -9295,361 +9272,30 @@
         <f>1-0.00185361577622313</f>
         <v>0.99814638422377688</v>
       </c>
-      <c r="L30" s="28" t="s">
+      <c r="L30" t="s">
         <v>47</v>
       </c>
       <c r="M30">
         <v>0.6908945686900958</v>
       </c>
-      <c r="N30" s="28" t="s">
+      <c r="N30" t="s">
         <v>49</v>
       </c>
-      <c r="P30" s="28">
+      <c r="P30">
         <f t="shared" si="6"/>
         <v>4252</v>
       </c>
-      <c r="Q30" s="28">
+      <c r="Q30">
         <f t="shared" si="7"/>
         <v>2674.0341633354983</v>
       </c>
-      <c r="R30" s="28">
+      <c r="R30">
         <f t="shared" si="8"/>
         <v>11858.514376996804</v>
       </c>
-      <c r="S30" s="28">
+      <c r="S30">
         <f t="shared" si="5"/>
         <v>18784.548540332304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B32" s="24"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="28">
-        <v>2010</v>
-      </c>
-      <c r="B33" s="28">
-        <v>1200.6513499999901</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="28">
-        <v>2011</v>
-      </c>
-      <c r="B34" s="28">
-        <v>2534.3001088299902</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="28">
-        <v>2012</v>
-      </c>
-      <c r="B35" s="28">
-        <v>2534.3001088299902</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="28">
-        <v>2013</v>
-      </c>
-      <c r="B36" s="28">
-        <v>5123.0323208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="28">
-        <v>2014</v>
-      </c>
-      <c r="B37" s="28">
-        <v>5123.0323208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="28">
-        <v>2015</v>
-      </c>
-      <c r="B38" s="28">
-        <v>9477.5425046750006</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="28">
-        <v>2016</v>
-      </c>
-      <c r="B39" s="28">
-        <v>9477.5425046750006</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="28">
-        <v>2017</v>
-      </c>
-      <c r="B40" s="28">
-        <v>9156.77890338</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="28">
-        <v>2018</v>
-      </c>
-      <c r="B41" s="28">
-        <v>9156.77890338</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="28">
-        <v>2019</v>
-      </c>
-      <c r="B42" s="28">
-        <v>16995.842998245</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="28">
-        <v>2020</v>
-      </c>
-      <c r="B43" s="28">
-        <v>16995.842998245</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="28">
-        <v>2021</v>
-      </c>
-      <c r="B44" s="28">
-        <v>4723.5930226999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="28">
-        <v>2022</v>
-      </c>
-      <c r="B45" s="28">
-        <v>4723.5930226999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="28">
-        <v>2023</v>
-      </c>
-      <c r="B46" s="28">
-        <v>34173.144328415001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="28">
-        <v>2024</v>
-      </c>
-      <c r="B47" s="28">
-        <v>34173.144328415001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="28">
-        <v>2025</v>
-      </c>
-      <c r="B48" s="28">
-        <v>73232.04575818</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="28">
-        <v>2026</v>
-      </c>
-      <c r="B49" s="28">
-        <v>73232.04575818</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="28">
-        <v>2027</v>
-      </c>
-      <c r="B50" s="28">
-        <v>61963.949007384901</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="28">
-        <v>2028</v>
-      </c>
-      <c r="B51" s="28">
-        <v>61963.949007384901</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="28">
-        <v>2029</v>
-      </c>
-      <c r="B52" s="28">
-        <v>81314.849570865001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="28">
-        <v>2030</v>
-      </c>
-      <c r="B53" s="28">
-        <v>81314.849570865001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="28">
-        <v>2031</v>
-      </c>
-      <c r="B54" s="28">
-        <v>49200.342204749999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="28">
-        <v>2032</v>
-      </c>
-      <c r="B55" s="28">
-        <v>49200.342204749999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="28">
-        <v>2033</v>
-      </c>
-      <c r="B56" s="28">
-        <v>100734.892095405</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="28">
-        <v>2034</v>
-      </c>
-      <c r="B57" s="28">
-        <v>100734.892095405</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="28">
-        <v>2035</v>
-      </c>
-      <c r="B58" s="28">
-        <v>89886.844265459993</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="28">
-        <v>2036</v>
-      </c>
-      <c r="B59" s="28">
-        <v>89886.844265459993</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="28">
-        <v>2037</v>
-      </c>
-      <c r="B60" s="28">
-        <v>59996.065785354898</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="28">
-        <v>2038</v>
-      </c>
-      <c r="B61" s="28">
-        <v>59996.065785354898</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="28">
-        <v>2039</v>
-      </c>
-      <c r="B62" s="28">
-        <v>13613.503684885</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="28">
-        <v>2040</v>
-      </c>
-      <c r="B63" s="28">
-        <v>13613.503684885</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="28">
-        <v>2041</v>
-      </c>
-      <c r="B64" s="28">
-        <v>36887.263406979997</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="28">
-        <v>2042</v>
-      </c>
-      <c r="B65" s="28">
-        <v>36887.263406979997</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="28">
-        <v>2043</v>
-      </c>
-      <c r="B66" s="28">
-        <v>44331.142776660003</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="28">
-        <v>2044</v>
-      </c>
-      <c r="B67" s="28">
-        <v>44331.142776660003</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="28">
-        <v>2045</v>
-      </c>
-      <c r="B68" s="28">
-        <v>71991.796050289995</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="28">
-        <v>2046</v>
-      </c>
-      <c r="B69" s="28">
-        <v>71991.796050289995</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="28">
-        <v>2047</v>
-      </c>
-      <c r="B70" s="28">
-        <v>42648.336863959899</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="28">
-        <v>2048</v>
-      </c>
-      <c r="B71" s="28">
-        <v>42648.336863959899</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="28">
-        <v>2049</v>
-      </c>
-      <c r="B72" s="28">
-        <v>69993.457237224997</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="28">
-        <v>2050</v>
-      </c>
-      <c r="B73" s="28">
-        <v>69993.457237224997</v>
       </c>
     </row>
   </sheetData>
@@ -9674,6 +9320,350 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BE2031-B992-49E6-B55B-44F4BF59B4D8}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2010</v>
+      </c>
+      <c r="B1">
+        <v>1200.6513499999901</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2011</v>
+      </c>
+      <c r="B2">
+        <v>2534.3001088299902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2012</v>
+      </c>
+      <c r="B3">
+        <v>2534.3001088299902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2013</v>
+      </c>
+      <c r="B4">
+        <v>5123.0323208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>5123.0323208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2015</v>
+      </c>
+      <c r="B6">
+        <v>9477.5425046750006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2016</v>
+      </c>
+      <c r="B7">
+        <v>9477.5425046750006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2017</v>
+      </c>
+      <c r="B8">
+        <v>9156.77890338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2018</v>
+      </c>
+      <c r="B9">
+        <v>9156.77890338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>16995.842998245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2020</v>
+      </c>
+      <c r="B11">
+        <v>16995.842998245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2021</v>
+      </c>
+      <c r="B12">
+        <v>4723.5930226999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2022</v>
+      </c>
+      <c r="B13">
+        <v>4723.5930226999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2023</v>
+      </c>
+      <c r="B14">
+        <v>34173.144328415001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2024</v>
+      </c>
+      <c r="B15">
+        <v>34173.144328415001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2025</v>
+      </c>
+      <c r="B16">
+        <v>73232.04575818</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2026</v>
+      </c>
+      <c r="B17">
+        <v>73232.04575818</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2027</v>
+      </c>
+      <c r="B18">
+        <v>61963.949007384901</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2028</v>
+      </c>
+      <c r="B19">
+        <v>61963.949007384901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2029</v>
+      </c>
+      <c r="B20">
+        <v>81314.849570865001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2030</v>
+      </c>
+      <c r="B21">
+        <v>81314.849570865001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2031</v>
+      </c>
+      <c r="B22">
+        <v>49200.342204749999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2032</v>
+      </c>
+      <c r="B23">
+        <v>49200.342204749999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2033</v>
+      </c>
+      <c r="B24">
+        <v>100734.892095405</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2034</v>
+      </c>
+      <c r="B25">
+        <v>100734.892095405</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2035</v>
+      </c>
+      <c r="B26">
+        <v>89886.844265459993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2036</v>
+      </c>
+      <c r="B27">
+        <v>89886.844265459993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2037</v>
+      </c>
+      <c r="B28">
+        <v>59996.065785354898</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2038</v>
+      </c>
+      <c r="B29">
+        <v>59996.065785354898</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2039</v>
+      </c>
+      <c r="B30">
+        <v>13613.503684885</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2040</v>
+      </c>
+      <c r="B31">
+        <v>13613.503684885</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2041</v>
+      </c>
+      <c r="B32">
+        <v>36887.263406979997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2042</v>
+      </c>
+      <c r="B33">
+        <v>36887.263406979997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2043</v>
+      </c>
+      <c r="B34">
+        <v>44331.142776660003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2044</v>
+      </c>
+      <c r="B35">
+        <v>44331.142776660003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2045</v>
+      </c>
+      <c r="B36">
+        <v>71991.796050289995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2046</v>
+      </c>
+      <c r="B37">
+        <v>71991.796050289995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>2047</v>
+      </c>
+      <c r="B38">
+        <v>42648.336863959899</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2048</v>
+      </c>
+      <c r="B39">
+        <v>42648.336863959899</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2049</v>
+      </c>
+      <c r="B40">
+        <v>69993.457237224997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>2050</v>
+      </c>
+      <c r="B41">
+        <v>69993.457237224997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68613016-2799-46F8-A7F1-1692A33A287D}">
   <dimension ref="A1:AT51"/>
   <sheetViews>
@@ -9715,7 +9705,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>34</v>
       </c>
       <c r="F1" t="s">
@@ -9744,23 +9734,23 @@
       <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="22" t="s">
+      <c r="X2" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="Y2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="30" t="s">
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AK2" t="s">
         <v>52</v>
       </c>
@@ -9841,34 +9831,34 @@
       <c r="X3" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="23" t="s">
+      <c r="Y3" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="Z3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="AA3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AB3" s="23" t="s">
+      <c r="AB3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AC3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AD3" s="27" t="s">
+      <c r="AD3" t="s">
         <v>36</v>
       </c>
-      <c r="AE3" s="27" t="s">
+      <c r="AE3" t="s">
         <v>37</v>
       </c>
-      <c r="AF3" s="27" t="s">
+      <c r="AF3" t="s">
         <v>40</v>
       </c>
-      <c r="AG3" s="27" t="s">
+      <c r="AG3" t="s">
         <v>38</v>
       </c>
-      <c r="AH3" s="27" t="s">
+      <c r="AH3" t="s">
         <v>31</v>
       </c>
       <c r="AI3" t="s">
@@ -9910,22 +9900,22 @@
         <v>1995</v>
       </c>
       <c r="P4" s="4"/>
-      <c r="X4" s="22">
+      <c r="X4">
         <v>12.5</v>
       </c>
-      <c r="Y4" s="23">
+      <c r="Y4" s="22">
         <v>19.3</v>
       </c>
-      <c r="Z4" s="23">
+      <c r="Z4" s="22">
         <v>25.8</v>
       </c>
-      <c r="AA4" s="23">
+      <c r="AA4" s="22">
         <v>9.6999999999999993</v>
       </c>
-      <c r="AB4" s="23">
+      <c r="AB4" s="22">
         <v>12</v>
       </c>
-      <c r="AC4" s="23">
+      <c r="AC4" s="22">
         <f>SUM(Y4:AB4)</f>
         <v>66.8</v>
       </c>
@@ -9933,19 +9923,19 @@
         <f>Y4</f>
         <v>19.3</v>
       </c>
-      <c r="AE4" s="27">
+      <c r="AE4">
         <f t="shared" ref="AE4:AG4" si="0">Z4</f>
         <v>25.8</v>
       </c>
-      <c r="AF4" s="27">
+      <c r="AF4">
         <f t="shared" si="0"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="AG4" s="27">
+      <c r="AG4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AH4" s="27">
+      <c r="AH4">
         <f>SUM(AD4:AG4)</f>
         <v>66.8</v>
       </c>
@@ -9963,22 +9953,22 @@
         <v>1996</v>
       </c>
       <c r="P5" s="4"/>
-      <c r="X5" s="22">
+      <c r="X5">
         <v>9.6999999999999993</v>
       </c>
-      <c r="Y5" s="23">
+      <c r="Y5" s="22">
         <v>23.3</v>
       </c>
-      <c r="Z5" s="23">
+      <c r="Z5" s="22">
         <v>30.2</v>
       </c>
-      <c r="AA5" s="23">
+      <c r="AA5" s="22">
         <v>11</v>
       </c>
-      <c r="AB5" s="23">
+      <c r="AB5" s="22">
         <v>12</v>
       </c>
-      <c r="AC5" s="23">
+      <c r="AC5" s="22">
         <f t="shared" ref="AC5:AC19" si="1">SUM(Y5:AB5)</f>
         <v>76.5</v>
       </c>
@@ -9986,23 +9976,23 @@
         <f>Y5-Y4</f>
         <v>4</v>
       </c>
-      <c r="AE5" s="27">
+      <c r="AE5">
         <f>Z5-Z4</f>
         <v>4.3999999999999986</v>
       </c>
-      <c r="AF5" s="27">
+      <c r="AF5">
         <f>AA5-AA4</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="AG5" s="27">
+      <c r="AG5">
         <f>AB5-AB4</f>
         <v>0</v>
       </c>
-      <c r="AH5" s="27">
+      <c r="AH5">
         <f t="shared" ref="AH5:AH19" si="2">SUM(AD5:AG5)</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="AI5" s="27">
+      <c r="AI5">
         <f t="shared" ref="AI5:AI19" si="3">SUM(AF5:AG5)</f>
         <v>1.3000000000000007</v>
       </c>
@@ -10016,46 +10006,46 @@
         <v>1997</v>
       </c>
       <c r="P6" s="4"/>
-      <c r="X6" s="22">
+      <c r="X6">
         <v>11.7</v>
       </c>
-      <c r="Y6" s="23">
+      <c r="Y6" s="22">
         <v>27.5</v>
       </c>
-      <c r="Z6" s="23">
+      <c r="Z6" s="22">
         <v>35</v>
       </c>
-      <c r="AA6" s="23">
+      <c r="AA6" s="22">
         <v>13.7</v>
       </c>
-      <c r="AB6" s="23">
+      <c r="AB6" s="22">
         <v>12</v>
       </c>
-      <c r="AC6" s="23">
+      <c r="AC6" s="22">
         <f t="shared" si="1"/>
         <v>88.2</v>
       </c>
-      <c r="AD6" s="27">
+      <c r="AD6">
         <f t="shared" ref="AD6:AD17" si="5">Y6-Y5</f>
         <v>4.1999999999999993</v>
       </c>
-      <c r="AE6" s="27">
+      <c r="AE6">
         <f t="shared" ref="AE6:AE17" si="6">Z6-Z5</f>
         <v>4.8000000000000007</v>
       </c>
-      <c r="AF6" s="27">
+      <c r="AF6">
         <f t="shared" ref="AF6:AF19" si="7">AA6-AA5</f>
         <v>2.6999999999999993</v>
       </c>
-      <c r="AG6" s="27">
+      <c r="AG6">
         <f t="shared" ref="AG6:AG19" si="8">AB6-AB5</f>
         <v>0</v>
       </c>
-      <c r="AH6" s="27">
+      <c r="AH6">
         <f t="shared" si="2"/>
         <v>11.7</v>
       </c>
-      <c r="AI6" s="27">
+      <c r="AI6">
         <f t="shared" si="3"/>
         <v>2.6999999999999993</v>
       </c>
@@ -10069,46 +10059,46 @@
         <v>1998</v>
       </c>
       <c r="P7" s="4"/>
-      <c r="X7" s="22">
+      <c r="X7">
         <v>11.9</v>
       </c>
-      <c r="Y7" s="23">
+      <c r="Y7" s="22">
         <v>32</v>
       </c>
-      <c r="Z7" s="23">
+      <c r="Z7" s="22">
         <v>40.200000000000003</v>
       </c>
-      <c r="AA7" s="23">
+      <c r="AA7" s="22">
         <v>15.9</v>
       </c>
-      <c r="AB7" s="23">
+      <c r="AB7" s="22">
         <v>12</v>
       </c>
-      <c r="AC7" s="23">
+      <c r="AC7" s="22">
         <f t="shared" si="1"/>
         <v>100.10000000000001</v>
       </c>
-      <c r="AD7" s="27">
+      <c r="AD7">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="AE7" s="27">
+      <c r="AE7">
         <f t="shared" si="6"/>
         <v>5.2000000000000028</v>
       </c>
-      <c r="AF7" s="27">
+      <c r="AF7">
         <f t="shared" si="7"/>
         <v>2.2000000000000011</v>
       </c>
-      <c r="AG7" s="27">
+      <c r="AG7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH7" s="27">
+      <c r="AH7">
         <f t="shared" si="2"/>
         <v>11.900000000000004</v>
       </c>
-      <c r="AI7" s="27">
+      <c r="AI7">
         <f t="shared" si="3"/>
         <v>2.2000000000000011</v>
       </c>
@@ -10144,43 +10134,43 @@
         <f t="shared" ref="P8:P17" si="10">(M8+N8)/O8</f>
         <v>1</v>
       </c>
-      <c r="Y8" s="23">
+      <c r="Y8" s="22">
         <v>37.5</v>
       </c>
-      <c r="Z8" s="23">
+      <c r="Z8" s="22">
         <v>46.7</v>
       </c>
-      <c r="AA8" s="23">
+      <c r="AA8" s="22">
         <v>21.1</v>
       </c>
-      <c r="AB8" s="23">
+      <c r="AB8" s="22">
         <v>12</v>
       </c>
-      <c r="AC8" s="23">
+      <c r="AC8" s="22">
         <f t="shared" si="1"/>
         <v>117.30000000000001</v>
       </c>
-      <c r="AD8" s="27">
+      <c r="AD8">
         <f t="shared" si="5"/>
         <v>5.5</v>
       </c>
-      <c r="AE8" s="27">
+      <c r="AE8">
         <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
-      <c r="AF8" s="27">
+      <c r="AF8">
         <f t="shared" si="7"/>
         <v>5.2000000000000011</v>
       </c>
-      <c r="AG8" s="27">
+      <c r="AG8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH8" s="27">
+      <c r="AH8">
         <f t="shared" si="2"/>
         <v>17.200000000000003</v>
       </c>
-      <c r="AI8" s="27">
+      <c r="AI8">
         <f t="shared" si="3"/>
         <v>5.2000000000000011</v>
       </c>
@@ -10229,43 +10219,43 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Y9" s="23">
+      <c r="Y9" s="22">
         <v>43.5</v>
       </c>
-      <c r="Z9" s="23">
+      <c r="Z9" s="22">
         <v>55.2</v>
       </c>
-      <c r="AA9" s="23">
+      <c r="AA9" s="22">
         <v>28.1</v>
       </c>
-      <c r="AB9" s="23">
+      <c r="AB9" s="22">
         <v>12</v>
       </c>
-      <c r="AC9" s="23">
+      <c r="AC9" s="22">
         <f t="shared" si="1"/>
         <v>138.80000000000001</v>
       </c>
-      <c r="AD9" s="27">
+      <c r="AD9">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="AE9" s="27">
+      <c r="AE9">
         <f t="shared" si="6"/>
         <v>8.5</v>
       </c>
-      <c r="AF9" s="27">
+      <c r="AF9">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="AG9" s="27">
+      <c r="AG9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH9" s="27">
+      <c r="AH9">
         <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
-      <c r="AI9" s="27">
+      <c r="AI9">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -10316,43 +10306,43 @@
         <f t="shared" si="10"/>
         <v>0.52500000000000002</v>
       </c>
-      <c r="Y10" s="23">
+      <c r="Y10" s="22">
         <v>50.5</v>
       </c>
-      <c r="Z10" s="23">
+      <c r="Z10" s="22">
         <v>64.7</v>
       </c>
-      <c r="AA10" s="23">
+      <c r="AA10" s="22">
         <v>40.6</v>
       </c>
-      <c r="AB10" s="23">
+      <c r="AB10" s="22">
         <v>12</v>
       </c>
-      <c r="AC10" s="23">
+      <c r="AC10" s="22">
         <f t="shared" si="1"/>
         <v>167.8</v>
       </c>
-      <c r="AD10" s="27">
+      <c r="AD10">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="AE10" s="27">
+      <c r="AE10">
         <f t="shared" si="6"/>
         <v>9.5</v>
       </c>
-      <c r="AF10" s="27">
+      <c r="AF10">
         <f t="shared" si="7"/>
         <v>12.5</v>
       </c>
-      <c r="AG10" s="27">
+      <c r="AG10">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH10" s="27">
+      <c r="AH10">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="AI10" s="27">
+      <c r="AI10">
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
@@ -10403,43 +10393,43 @@
         <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
-      <c r="Y11" s="23">
+      <c r="Y11" s="22">
         <v>58.9</v>
       </c>
-      <c r="Z11" s="23">
+      <c r="Z11" s="22">
         <v>77.7</v>
       </c>
-      <c r="AA11" s="23">
+      <c r="AA11" s="22">
         <v>63.6</v>
       </c>
-      <c r="AB11" s="23">
+      <c r="AB11" s="22">
         <v>12</v>
       </c>
-      <c r="AC11" s="23">
+      <c r="AC11" s="22">
         <f t="shared" si="1"/>
         <v>212.2</v>
       </c>
-      <c r="AD11" s="27">
+      <c r="AD11">
         <f t="shared" si="5"/>
         <v>8.3999999999999986</v>
       </c>
-      <c r="AE11" s="27">
+      <c r="AE11">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="AF11" s="27">
+      <c r="AF11">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="AG11" s="27">
+      <c r="AG11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AH11" s="27">
+      <c r="AH11">
         <f t="shared" si="2"/>
         <v>44.4</v>
       </c>
-      <c r="AI11" s="27">
+      <c r="AI11">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
@@ -10490,43 +10480,43 @@
         <f t="shared" si="10"/>
         <v>0.65938864628820959</v>
       </c>
-      <c r="Y12" s="23">
+      <c r="Y12" s="22">
         <v>67.900000000000006</v>
       </c>
-      <c r="Z12" s="23">
+      <c r="Z12" s="22">
         <v>93.7</v>
       </c>
-      <c r="AA12" s="23">
+      <c r="AA12" s="22">
         <v>95.6</v>
       </c>
-      <c r="AB12" s="23">
+      <c r="AB12" s="22">
         <v>18</v>
       </c>
-      <c r="AC12" s="23">
+      <c r="AC12" s="22">
         <f t="shared" si="1"/>
         <v>275.20000000000005</v>
       </c>
-      <c r="AD12" s="27">
+      <c r="AD12">
         <f t="shared" si="5"/>
         <v>9.0000000000000071</v>
       </c>
-      <c r="AE12" s="27">
+      <c r="AE12">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="AF12" s="27">
+      <c r="AF12">
         <f t="shared" si="7"/>
         <v>31.999999999999993</v>
       </c>
-      <c r="AG12" s="27">
+      <c r="AG12">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="AH12" s="27">
+      <c r="AH12">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="AI12" s="27">
+      <c r="AI12">
         <f t="shared" si="3"/>
         <v>37.999999999999993</v>
       </c>
@@ -10577,43 +10567,43 @@
         <f t="shared" si="10"/>
         <v>0.57612456747404839</v>
       </c>
-      <c r="Y13" s="23">
+      <c r="Y13" s="22">
         <v>88</v>
       </c>
-      <c r="Z13" s="23">
+      <c r="Z13" s="22">
         <v>112</v>
       </c>
-      <c r="AA13" s="23">
+      <c r="AA13" s="22">
         <v>154</v>
       </c>
-      <c r="AB13" s="23">
+      <c r="AB13" s="22">
         <v>22</v>
       </c>
-      <c r="AC13" s="23">
+      <c r="AC13" s="22">
         <f t="shared" si="1"/>
         <v>376</v>
       </c>
-      <c r="AD13" s="27">
+      <c r="AD13">
         <f t="shared" si="5"/>
         <v>20.099999999999994</v>
       </c>
-      <c r="AE13" s="27">
+      <c r="AE13">
         <f t="shared" si="6"/>
         <v>18.299999999999997</v>
       </c>
-      <c r="AF13" s="27">
+      <c r="AF13">
         <f t="shared" si="7"/>
         <v>58.400000000000006</v>
       </c>
-      <c r="AG13" s="27">
+      <c r="AG13">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="AH13" s="27">
+      <c r="AH13">
         <f t="shared" si="2"/>
         <v>100.8</v>
       </c>
-      <c r="AI13" s="27">
+      <c r="AI13">
         <f t="shared" si="3"/>
         <v>62.400000000000006</v>
       </c>
@@ -10664,43 +10654,43 @@
         <f t="shared" si="10"/>
         <v>0.64885496183206104</v>
       </c>
-      <c r="Y14" s="23">
+      <c r="Y14" s="22">
         <v>100</v>
       </c>
-      <c r="Z14" s="23">
+      <c r="Z14" s="22">
         <v>133</v>
       </c>
-      <c r="AA14" s="23">
+      <c r="AA14" s="22">
         <v>219</v>
       </c>
-      <c r="AB14" s="23">
+      <c r="AB14" s="22">
         <v>27</v>
       </c>
-      <c r="AC14" s="23">
+      <c r="AC14" s="22">
         <f t="shared" si="1"/>
         <v>479</v>
       </c>
-      <c r="AD14" s="27">
+      <c r="AD14">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="AE14" s="27">
+      <c r="AE14">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="AF14" s="27">
+      <c r="AF14">
         <f t="shared" si="7"/>
         <v>65</v>
       </c>
-      <c r="AG14" s="27">
+      <c r="AG14">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="AH14" s="27">
+      <c r="AH14">
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
-      <c r="AI14" s="27">
+      <c r="AI14">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
@@ -10751,43 +10741,43 @@
         <f t="shared" si="10"/>
         <v>0.64011516314779271</v>
       </c>
-      <c r="Y15" s="23">
+      <c r="Y15" s="22">
         <v>114</v>
       </c>
-      <c r="Z15" s="25">
+      <c r="Z15" s="24">
         <v>155</v>
       </c>
-      <c r="AA15" s="23">
+      <c r="AA15" s="22">
         <v>322</v>
       </c>
-      <c r="AB15" s="23">
+      <c r="AB15" s="22">
         <v>32</v>
       </c>
-      <c r="AC15" s="23">
+      <c r="AC15" s="22">
         <f t="shared" si="1"/>
         <v>623</v>
       </c>
-      <c r="AD15" s="27">
+      <c r="AD15">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="AE15" s="27">
+      <c r="AE15">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="AF15" s="27">
+      <c r="AF15">
         <f t="shared" si="7"/>
         <v>103</v>
       </c>
-      <c r="AG15" s="27">
+      <c r="AG15">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="AH15" s="27">
+      <c r="AH15">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="AI15" s="27">
+      <c r="AI15">
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
@@ -10841,43 +10831,43 @@
         <f t="shared" si="10"/>
         <v>0.63965087281795519</v>
       </c>
-      <c r="Y16" s="23">
+      <c r="Y16" s="22">
         <v>134</v>
       </c>
-      <c r="Z16" s="23">
+      <c r="Z16" s="22">
         <v>191</v>
       </c>
-      <c r="AA16" s="23">
+      <c r="AA16" s="22">
         <v>465</v>
       </c>
-      <c r="AB16" s="23">
+      <c r="AB16" s="22">
         <v>40.5</v>
       </c>
-      <c r="AC16" s="23">
+      <c r="AC16" s="22">
         <f t="shared" si="1"/>
         <v>830.5</v>
       </c>
-      <c r="AD16" s="27">
+      <c r="AD16">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="AE16" s="27">
+      <c r="AE16">
         <f t="shared" si="6"/>
         <v>36</v>
       </c>
-      <c r="AF16" s="27">
+      <c r="AF16">
         <f t="shared" si="7"/>
         <v>143</v>
       </c>
-      <c r="AG16" s="27">
+      <c r="AG16">
         <f t="shared" si="8"/>
         <v>8.5</v>
       </c>
-      <c r="AH16" s="27">
+      <c r="AH16">
         <f t="shared" si="2"/>
         <v>207.5</v>
       </c>
-      <c r="AI16" s="27">
+      <c r="AI16">
         <f t="shared" si="3"/>
         <v>151.5</v>
       </c>
@@ -10963,43 +10953,43 @@
         <f t="shared" si="10"/>
         <v>0.7325060324026198</v>
       </c>
-      <c r="Y17" s="23">
+      <c r="Y17" s="22">
         <v>154</v>
       </c>
-      <c r="Z17" s="23">
+      <c r="Z17" s="22">
         <v>216</v>
       </c>
-      <c r="AA17" s="23">
+      <c r="AA17" s="22">
         <v>735</v>
       </c>
-      <c r="AB17" s="23">
+      <c r="AB17" s="22">
         <v>63.5</v>
       </c>
-      <c r="AC17" s="23">
+      <c r="AC17" s="22">
         <f t="shared" si="1"/>
         <v>1168.5</v>
       </c>
-      <c r="AD17" s="27">
+      <c r="AD17">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="AE17" s="27">
+      <c r="AE17">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="AF17" s="27">
+      <c r="AF17">
         <f t="shared" si="7"/>
         <v>270</v>
       </c>
-      <c r="AG17" s="27">
+      <c r="AG17">
         <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="AH17" s="27">
+      <c r="AH17">
         <f t="shared" si="2"/>
         <v>338</v>
       </c>
-      <c r="AI17" s="27">
+      <c r="AI17">
         <f t="shared" si="3"/>
         <v>293</v>
       </c>
@@ -11022,11 +11012,11 @@
       <c r="AO17">
         <v>0.01</v>
       </c>
-      <c r="AP17" s="28">
+      <c r="AP17">
         <f t="shared" ref="AP17:AP30" si="13">(AN17+AO17)*1000</f>
         <v>10</v>
       </c>
-      <c r="AQ17" s="28">
+      <c r="AQ17">
         <f t="shared" ref="AQ17:AQ30" si="14">AP17/AM17</f>
         <v>0.46511627906976744</v>
       </c>
@@ -11110,38 +11100,38 @@
         <f>V18/SUM(Q18,V18)</f>
         <v>0.64164810690423169</v>
       </c>
-      <c r="Y18" s="31">
+      <c r="Y18" s="28">
         <v>400</v>
       </c>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="23">
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="22">
         <v>1103.5999999999999</v>
       </c>
-      <c r="AB18" s="23">
+      <c r="AB18" s="22">
         <v>130</v>
       </c>
-      <c r="AC18" s="23">
+      <c r="AC18" s="22">
         <f t="shared" si="1"/>
         <v>1633.6</v>
       </c>
-      <c r="AD18" s="30">
+      <c r="AD18" s="27">
         <f>Y18-(AD17+AE17)</f>
         <v>355</v>
       </c>
-      <c r="AE18" s="30"/>
-      <c r="AF18" s="27">
+      <c r="AE18" s="27"/>
+      <c r="AF18">
         <f t="shared" si="7"/>
         <v>368.59999999999991</v>
       </c>
-      <c r="AG18" s="27">
+      <c r="AG18">
         <f t="shared" si="8"/>
         <v>66.5</v>
       </c>
-      <c r="AH18" s="27">
+      <c r="AH18">
         <f t="shared" si="2"/>
         <v>790.09999999999991</v>
       </c>
-      <c r="AI18" s="27">
+      <c r="AI18">
         <f t="shared" si="3"/>
         <v>435.09999999999991</v>
       </c>
@@ -11164,11 +11154,11 @@
       <c r="AO18">
         <v>0.02</v>
       </c>
-      <c r="AP18" s="28">
+      <c r="AP18">
         <f t="shared" si="13"/>
         <v>40</v>
       </c>
-      <c r="AQ18" s="28">
+      <c r="AQ18">
         <f t="shared" si="14"/>
         <v>0.57553956834532372</v>
       </c>
@@ -11237,38 +11227,38 @@
         <f>V19/SUM(Q19,V19)</f>
         <v>0.70660694288913772</v>
       </c>
-      <c r="Y19" s="31">
+      <c r="Y19" s="28">
         <v>440</v>
       </c>
-      <c r="Z19" s="31"/>
-      <c r="AA19" s="23">
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="22">
         <v>1737</v>
       </c>
-      <c r="AB19" s="23">
+      <c r="AB19" s="22">
         <v>372</v>
       </c>
-      <c r="AC19" s="23">
+      <c r="AC19" s="22">
         <f t="shared" si="1"/>
         <v>2549</v>
       </c>
-      <c r="AD19" s="30">
+      <c r="AD19" s="27">
         <f>Y19-AD18</f>
         <v>85</v>
       </c>
-      <c r="AE19" s="30"/>
-      <c r="AF19" s="27">
+      <c r="AE19" s="27"/>
+      <c r="AF19">
         <f t="shared" si="7"/>
         <v>633.40000000000009</v>
       </c>
-      <c r="AG19" s="27">
+      <c r="AG19">
         <f t="shared" si="8"/>
         <v>242</v>
       </c>
-      <c r="AH19" s="27">
+      <c r="AH19">
         <f t="shared" si="2"/>
         <v>960.40000000000009</v>
       </c>
-      <c r="AI19" s="27">
+      <c r="AI19">
         <f t="shared" si="3"/>
         <v>875.40000000000009</v>
       </c>
@@ -11276,13 +11266,13 @@
         <f t="shared" si="4"/>
         <v>0.91149521032902958</v>
       </c>
-      <c r="AK19" s="29">
+      <c r="AK19" s="26">
         <v>245.53688562500002</v>
       </c>
-      <c r="AL19" s="29">
+      <c r="AL19" s="26">
         <v>336.80107500000008</v>
       </c>
-      <c r="AM19" s="29">
+      <c r="AM19" s="26">
         <v>266.5</v>
       </c>
       <c r="AN19">
@@ -11291,11 +11281,11 @@
       <c r="AO19">
         <v>0.12</v>
       </c>
-      <c r="AP19" s="28">
+      <c r="AP19">
         <f t="shared" si="13"/>
         <v>180</v>
       </c>
-      <c r="AQ19" s="28">
+      <c r="AQ19">
         <f t="shared" si="14"/>
         <v>0.67542213883677293</v>
       </c>
@@ -11364,15 +11354,13 @@
         <f>V20/SUM(Q20,V20)</f>
         <v>0.824295010845987</v>
       </c>
-      <c r="AI20" s="27"/>
-      <c r="AJ20" s="27"/>
-      <c r="AK20" s="29">
+      <c r="AK20" s="26">
         <v>305.17506160499994</v>
       </c>
-      <c r="AL20" s="29">
+      <c r="AL20" s="26">
         <v>849.96753279699988</v>
       </c>
-      <c r="AM20" s="29">
+      <c r="AM20" s="26">
         <v>785.59460999999988</v>
       </c>
       <c r="AN20">
@@ -11381,11 +11369,11 @@
       <c r="AO20">
         <v>0.12</v>
       </c>
-      <c r="AP20" s="28">
+      <c r="AP20">
         <f t="shared" si="13"/>
         <v>480</v>
       </c>
-      <c r="AQ20" s="28">
+      <c r="AQ20">
         <f t="shared" si="14"/>
         <v>0.61100215542466629</v>
       </c>
@@ -11460,15 +11448,13 @@
         <f>V21/SUM(Q21,V21)</f>
         <v>0.84659732885244954</v>
       </c>
-      <c r="AI21" s="27"/>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="29">
+      <c r="AK21" s="26">
         <v>495.52947265229875</v>
       </c>
-      <c r="AL21" s="29">
+      <c r="AL21" s="26">
         <v>1075.1495344149428</v>
       </c>
-      <c r="AM21" s="29">
+      <c r="AM21" s="26">
         <v>1803.1759999999997</v>
       </c>
       <c r="AN21">
@@ -11477,11 +11463,11 @@
       <c r="AO21">
         <v>0.23</v>
       </c>
-      <c r="AP21" s="28">
+      <c r="AP21">
         <f t="shared" si="13"/>
         <v>929.99999999999989</v>
       </c>
-      <c r="AQ21" s="28">
+      <c r="AQ21">
         <f t="shared" si="14"/>
         <v>0.51575664272372745</v>
       </c>
@@ -11540,15 +11526,13 @@
         <f>V22/SUM(Q22,V22)</f>
         <v>0.80580848401156524</v>
       </c>
-      <c r="AI22" s="27"/>
-      <c r="AJ22" s="27"/>
-      <c r="AK22" s="29">
+      <c r="AK22" s="26">
         <v>798.95041698643684</v>
       </c>
-      <c r="AL22" s="29">
+      <c r="AL22" s="26">
         <v>1109.3416131057468</v>
       </c>
-      <c r="AM22" s="29">
+      <c r="AM22" s="26">
         <v>2857.5100000000007</v>
       </c>
       <c r="AN22">
@@ -11557,11 +11541,11 @@
       <c r="AO22">
         <v>0.5</v>
       </c>
-      <c r="AP22" s="28">
+      <c r="AP22">
         <f t="shared" si="13"/>
         <v>1350</v>
       </c>
-      <c r="AQ22" s="28">
+      <c r="AQ22">
         <f t="shared" si="14"/>
         <v>0.47243929155103559</v>
       </c>
@@ -11604,15 +11588,13 @@
       <c r="S23" t="s">
         <v>12</v>
       </c>
-      <c r="AI23" s="27"/>
-      <c r="AJ23" s="27"/>
-      <c r="AK23" s="29">
+      <c r="AK23" s="26">
         <v>1267.7345639544415</v>
       </c>
-      <c r="AL23" s="29">
+      <c r="AL23" s="26">
         <v>1055.1740047974631</v>
       </c>
-      <c r="AM23" s="29">
+      <c r="AM23" s="26">
         <v>3921.9410000000003</v>
       </c>
       <c r="AN23">
@@ -11621,11 +11603,11 @@
       <c r="AO23">
         <v>2.2200000000000002</v>
       </c>
-      <c r="AP23" s="28">
+      <c r="AP23">
         <f t="shared" si="13"/>
         <v>3170</v>
       </c>
-      <c r="AQ23" s="28">
+      <c r="AQ23">
         <f t="shared" si="14"/>
         <v>0.80827325041350695</v>
       </c>
@@ -11659,15 +11641,13 @@
         <f t="shared" si="17"/>
         <v>0.70895614431880372</v>
       </c>
-      <c r="AI24" s="27"/>
-      <c r="AJ24" s="27"/>
-      <c r="AK24" s="29">
+      <c r="AK24" s="26">
         <v>2171.3991644181156</v>
       </c>
-      <c r="AL24" s="29">
+      <c r="AL24" s="26">
         <v>1069.6787157635285</v>
       </c>
-      <c r="AM24" s="29">
+      <c r="AM24" s="26">
         <v>4267.9800000000014</v>
       </c>
       <c r="AN24">
@@ -11676,11 +11656,11 @@
       <c r="AO24">
         <v>0.54</v>
       </c>
-      <c r="AP24" s="28">
+      <c r="AP24">
         <f t="shared" si="13"/>
         <v>2870</v>
       </c>
-      <c r="AQ24" s="28">
+      <c r="AQ24">
         <f t="shared" si="14"/>
         <v>0.67244926171162922</v>
       </c>
@@ -11714,15 +11694,13 @@
         <f t="shared" si="17"/>
         <v>0.82259236143177517</v>
       </c>
-      <c r="AI25" s="27"/>
-      <c r="AJ25" s="27"/>
-      <c r="AK25" s="29">
+      <c r="AK25" s="26">
         <v>2638.4647128689089</v>
       </c>
-      <c r="AL25" s="29">
+      <c r="AL25" s="26">
         <v>1714.8479983645557</v>
       </c>
-      <c r="AM25" s="29">
+      <c r="AM25" s="26">
         <v>10750.848425702876</v>
       </c>
       <c r="AN25">
@@ -11731,11 +11709,11 @@
       <c r="AO25">
         <v>1.73</v>
       </c>
-      <c r="AP25" s="28">
+      <c r="AP25">
         <f t="shared" si="13"/>
         <v>7439.9999999999991</v>
       </c>
-      <c r="AQ25" s="28">
+      <c r="AQ25">
         <f t="shared" si="14"/>
         <v>0.69203840528647231</v>
       </c>
@@ -11769,15 +11747,13 @@
         <f t="shared" si="17"/>
         <v>0.78687254978114662</v>
       </c>
-      <c r="AI26" s="27"/>
-      <c r="AJ26" s="27"/>
-      <c r="AK26" s="29">
+      <c r="AK26" s="26">
         <v>2239.1755139334964</v>
       </c>
-      <c r="AL26" s="29">
+      <c r="AL26" s="26">
         <v>2365.7083752786466</v>
       </c>
-      <c r="AM26" s="29">
+      <c r="AM26" s="26">
         <v>6475.5621763345271</v>
       </c>
       <c r="AN26">
@@ -11786,11 +11762,11 @@
       <c r="AO26">
         <v>0.91</v>
       </c>
-      <c r="AP26" s="28">
+      <c r="AP26">
         <f t="shared" si="13"/>
         <v>4080</v>
       </c>
-      <c r="AQ26" s="28">
+      <c r="AQ26">
         <f t="shared" si="14"/>
         <v>0.63006112657070834</v>
       </c>
@@ -11824,15 +11800,13 @@
         <f t="shared" si="17"/>
         <v>0.77328917803719699</v>
       </c>
-      <c r="AI27" s="27"/>
-      <c r="AJ27" s="27"/>
-      <c r="AK27" s="29">
+      <c r="AK27" s="26">
         <v>2418.298837433078</v>
       </c>
-      <c r="AL27" s="29">
+      <c r="AL27" s="26">
         <v>2196.1894898222545</v>
       </c>
-      <c r="AM27" s="29">
+      <c r="AM27" s="26">
         <v>6118.7750969831295</v>
       </c>
       <c r="AN27">
@@ -11841,11 +11815,11 @@
       <c r="AO27">
         <v>0.99</v>
       </c>
-      <c r="AP27" s="28">
+      <c r="AP27">
         <f t="shared" si="13"/>
         <v>3969.9999999999995</v>
       </c>
-      <c r="AQ27" s="28">
+      <c r="AQ27">
         <f t="shared" si="14"/>
         <v>0.64882267072659916</v>
       </c>
@@ -11879,15 +11853,13 @@
         <f t="shared" si="17"/>
         <v>0.77982783875477768</v>
       </c>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="27"/>
-      <c r="AK28" s="29">
+      <c r="AK28" s="26">
         <v>2865.3565608774225</v>
       </c>
-      <c r="AL28" s="29">
+      <c r="AL28" s="26">
         <v>2184.2594336236671</v>
       </c>
-      <c r="AM28" s="29">
+      <c r="AM28" s="26">
         <v>8462.2720382445132</v>
       </c>
       <c r="AN28">
@@ -11896,11 +11868,11 @@
       <c r="AO28">
         <v>1.64</v>
       </c>
-      <c r="AP28" s="28">
+      <c r="AP28">
         <f t="shared" si="13"/>
         <v>4610</v>
       </c>
-      <c r="AQ28" s="28">
+      <c r="AQ28">
         <f t="shared" si="14"/>
         <v>0.54477095266678977</v>
       </c>
@@ -11934,15 +11906,13 @@
         <f t="shared" si="17"/>
         <v>0.8239738534260812</v>
       </c>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="27"/>
-      <c r="AK29" s="29">
+      <c r="AK29" s="26">
         <v>3242.0179045716945</v>
       </c>
-      <c r="AL29" s="29">
+      <c r="AL29" s="26">
         <v>2346.87782841427</v>
       </c>
-      <c r="AM29" s="29">
+      <c r="AM29" s="26">
         <v>14260.581686776355</v>
       </c>
       <c r="AN29">
@@ -11951,11 +11921,11 @@
       <c r="AO29">
         <v>2.8</v>
       </c>
-      <c r="AP29" s="28">
+      <c r="AP29">
         <f t="shared" si="13"/>
         <v>9620.0000000000018</v>
       </c>
-      <c r="AQ29" s="28">
+      <c r="AQ29">
         <f t="shared" si="14"/>
         <v>0.67458678834401953</v>
       </c>
@@ -11989,15 +11959,13 @@
         <f t="shared" si="17"/>
         <v>0.82151828368770219</v>
       </c>
-      <c r="AI30" s="27"/>
-      <c r="AJ30" s="27"/>
-      <c r="AK30" s="29">
+      <c r="AK30" s="26">
         <v>4205.8553926871946</v>
       </c>
-      <c r="AL30" s="29">
+      <c r="AL30" s="26">
         <v>2392.3642414796768</v>
       </c>
-      <c r="AM30" s="29">
+      <c r="AM30" s="26">
         <v>16966.409166959249</v>
       </c>
       <c r="AN30">
@@ -12006,11 +11974,11 @@
       <c r="AO30">
         <v>3.87</v>
       </c>
-      <c r="AP30" s="28">
+      <c r="AP30">
         <f t="shared" si="13"/>
         <v>12520</v>
       </c>
-      <c r="AQ30" s="28">
+      <c r="AQ30">
         <f t="shared" si="14"/>
         <v>0.73792868466132</v>
       </c>

</xml_diff>